<commit_message>
put libraries at the top of the list in Berrie
</commit_message>
<xml_diff>
--- a/Web Scraping/choco.xlsx
+++ b/Web Scraping/choco.xlsx
@@ -8,6 +8,7 @@
   </bookViews>
   <sheets>
     <sheet name="Sheet" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="AH_Choco" sheetId="2" state="visible" r:id="rId2"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -413,7 +414,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G35"/>
+  <dimension ref="A1:G99"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -491,7 +492,7 @@
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>2025-03-24</t>
+          <t>2025-03-31</t>
         </is>
       </c>
     </row>
@@ -528,7 +529,7 @@
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>2025-03-24</t>
+          <t>2025-03-31</t>
         </is>
       </c>
     </row>
@@ -565,7 +566,7 @@
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>2025-03-24</t>
+          <t>2025-03-31</t>
         </is>
       </c>
     </row>
@@ -602,14 +603,14 @@
       </c>
       <c r="G5" t="inlineStr">
         <is>
-          <t>2025-03-24</t>
+          <t>2025-03-31</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>Jumbo Paaseitjes Melk, Wit &amp; Puur Praliné Vulling 200 g</t>
+          <t>Jumbo Paaseitjes Witte Chocolade Massief 200 g</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
@@ -639,14 +640,14 @@
       </c>
       <c r="G6" t="inlineStr">
         <is>
-          <t>2025-03-24</t>
+          <t>2025-03-31</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>Jumbo Choco Pinda's 450 g</t>
+          <t>Jumbo Paaseitjes Melk Karamel Zeezout Massief 200 g</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
@@ -656,12 +657,12 @@
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>2,88</t>
+          <t>3,59</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>450 gram</t>
+          <t>200 g</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
@@ -676,14 +677,14 @@
       </c>
       <c r="G7" t="inlineStr">
         <is>
-          <t>2025-03-24</t>
+          <t>2025-03-31</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>Jumbo Paaseitjes Witte Chocolade Massief 200 g</t>
+          <t>Jumbo Paaseitjes Melk, Wit &amp; Puur Praliné Vulling 200 g</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
@@ -713,7 +714,7 @@
       </c>
       <c r="G8" t="inlineStr">
         <is>
-          <t>2025-03-24</t>
+          <t>2025-03-31</t>
         </is>
       </c>
     </row>
@@ -750,14 +751,14 @@
       </c>
       <c r="G9" t="inlineStr">
         <is>
-          <t>2025-03-24</t>
+          <t>2025-03-31</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>Jumbo Paaseitjes Melk Karamel Zeezout Massief 200 g</t>
+          <t>Jumbo Holle Paaseieren Melkchocolade 10 stuks</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
@@ -767,7 +768,7 @@
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>3,59</t>
+          <t>4,19</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
@@ -787,7 +788,7 @@
       </c>
       <c r="G10" t="inlineStr">
         <is>
-          <t>2025-03-24</t>
+          <t>2025-03-31</t>
         </is>
       </c>
     </row>
@@ -824,7 +825,7 @@
       </c>
       <c r="G11" t="inlineStr">
         <is>
-          <t>2025-03-24</t>
+          <t>2025-03-31</t>
         </is>
       </c>
     </row>
@@ -861,7 +862,7 @@
       </c>
       <c r="G12" t="inlineStr">
         <is>
-          <t>2025-03-24</t>
+          <t>2025-03-31</t>
         </is>
       </c>
     </row>
@@ -898,14 +899,14 @@
       </c>
       <c r="G13" t="inlineStr">
         <is>
-          <t>2025-03-24</t>
+          <t>2025-03-31</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>Jumbo Holle Paaseieren Melkchocolade 10 stuks</t>
+          <t>Jumbo Paaseitjes Melk Crème Brûléesmaak Vulling 200 g</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
@@ -915,7 +916,7 @@
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>4,19</t>
+          <t>3,59</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
@@ -935,14 +936,14 @@
       </c>
       <c r="G14" t="inlineStr">
         <is>
-          <t>2025-03-24</t>
+          <t>2025-03-31</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>Jumbo Paaseitjes Melk Praliné Vulling 200 g</t>
+          <t>Jumbo Paaseitjes Puur met Bossche Bol Smaak Vulling 200 g</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
@@ -972,14 +973,14 @@
       </c>
       <c r="G15" t="inlineStr">
         <is>
-          <t>2025-03-24</t>
+          <t>2025-03-31</t>
         </is>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>Jumbo Paaseitjes Melk met Nougat Vulling 200 g</t>
+          <t>Jumbo Paaseitjes Melk Praliné Vulling 200 g</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
@@ -1009,14 +1010,14 @@
       </c>
       <c r="G16" t="inlineStr">
         <is>
-          <t>2025-03-24</t>
+          <t>2025-03-31</t>
         </is>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>Jumbo Choco Rozijnen Melk 200 g</t>
+          <t>Jumbo Paaseitjes Stroopwafel Smaak Massief Melk 200 g</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
@@ -1026,7 +1027,7 @@
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>1,51</t>
+          <t>3,59</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
@@ -1046,14 +1047,14 @@
       </c>
       <c r="G17" t="inlineStr">
         <is>
-          <t>2025-03-24</t>
+          <t>2025-03-31</t>
         </is>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>Jumbo Paaseitjes Melk Karamel Vulling 200 g</t>
+          <t>Jumbo Paaseitjes Puur met Espresso Vulling 200 g</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
@@ -1083,14 +1084,14 @@
       </c>
       <c r="G18" t="inlineStr">
         <is>
-          <t>2025-03-24</t>
+          <t>2025-03-31</t>
         </is>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>Jumbo Paaseitjes Puur met Espresso Vulling 200 g</t>
+          <t>Jumbo Paaseitjes Melk Karamel Vulling 200 g</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
@@ -1120,14 +1121,14 @@
       </c>
       <c r="G19" t="inlineStr">
         <is>
-          <t>2025-03-24</t>
+          <t>2025-03-31</t>
         </is>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>Jumbo Paaseitjes Melk Crème Brûléesmaak Vulling 200 g</t>
+          <t>Jumbo Choco Rozijnen Melk 200 g</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
@@ -1137,7 +1138,7 @@
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>3,59</t>
+          <t>1,51</t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
@@ -1157,14 +1158,14 @@
       </c>
       <c r="G20" t="inlineStr">
         <is>
-          <t>2025-03-24</t>
+          <t>2025-03-31</t>
         </is>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>Jumbo Paaseitjes Stroopwafel Smaak Massief Melk 200 g</t>
+          <t>Jumbo Choco Classic 200 g</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
@@ -1174,7 +1175,7 @@
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>3,59</t>
+          <t>2,27</t>
         </is>
       </c>
       <c r="D21" t="inlineStr">
@@ -1194,14 +1195,14 @@
       </c>
       <c r="G21" t="inlineStr">
         <is>
-          <t>2025-03-24</t>
+          <t>2025-03-31</t>
         </is>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>Jumbo Choco Classic 200 g</t>
+          <t>Jumbo Chocolade Kuikens Wit 150 g</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
@@ -1211,12 +1212,12 @@
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>2,27</t>
+          <t>3,59</t>
         </is>
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>200 g</t>
+          <t>150 g</t>
         </is>
       </c>
       <c r="E22" t="inlineStr">
@@ -1231,7 +1232,7 @@
       </c>
       <c r="G22" t="inlineStr">
         <is>
-          <t>2025-03-24</t>
+          <t>2025-03-31</t>
         </is>
       </c>
     </row>
@@ -1268,7 +1269,7 @@
       </c>
       <c r="G23" t="inlineStr">
         <is>
-          <t>2025-03-24</t>
+          <t>2025-03-31</t>
         </is>
       </c>
     </row>
@@ -1305,14 +1306,14 @@
       </c>
       <c r="G24" t="inlineStr">
         <is>
-          <t>2025-03-24</t>
+          <t>2025-03-31</t>
         </is>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>Jumbo Paaseitjes Puur met Bossche Bol Smaak Vulling 200 g</t>
+          <t>Jumbo Paaseitjes Wit met Appeltaart Smaak Vulling 200 g</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
@@ -1342,7 +1343,7 @@
       </c>
       <c r="G25" t="inlineStr">
         <is>
-          <t>2025-03-24</t>
+          <t>2025-03-31</t>
         </is>
       </c>
     </row>
@@ -1379,7 +1380,7 @@
       </c>
       <c r="G26" t="inlineStr">
         <is>
-          <t>2025-03-24</t>
+          <t>2025-03-31</t>
         </is>
       </c>
     </row>
@@ -1394,7 +1395,6 @@
           <t>1.68</t>
         </is>
       </c>
-      <c r="C27" t="inlineStr"/>
       <c r="D27" t="inlineStr">
         <is>
           <t>Per 250 g</t>
@@ -1412,7 +1412,7 @@
       </c>
       <c r="G27" t="inlineStr">
         <is>
-          <t>2025-03-24</t>
+          <t>2025-03-31</t>
         </is>
       </c>
     </row>
@@ -1427,7 +1427,6 @@
           <t>2.39</t>
         </is>
       </c>
-      <c r="C28" t="inlineStr"/>
       <c r="D28" t="inlineStr">
         <is>
           <t>Per 200 g</t>
@@ -1445,7 +1444,7 @@
       </c>
       <c r="G28" t="inlineStr">
         <is>
-          <t>2025-03-24</t>
+          <t>2025-03-31</t>
         </is>
       </c>
     </row>
@@ -1460,7 +1459,6 @@
           <t>2.05</t>
         </is>
       </c>
-      <c r="C29" t="inlineStr"/>
       <c r="D29" t="inlineStr">
         <is>
           <t>Per 150 g</t>
@@ -1478,7 +1476,7 @@
       </c>
       <c r="G29" t="inlineStr">
         <is>
-          <t>2025-03-24</t>
+          <t>2025-03-31</t>
         </is>
       </c>
     </row>
@@ -1493,7 +1491,6 @@
           <t>2.49</t>
         </is>
       </c>
-      <c r="C30" t="inlineStr"/>
       <c r="D30" t="inlineStr">
         <is>
           <t>Per 210 g</t>
@@ -1511,7 +1508,7 @@
       </c>
       <c r="G30" t="inlineStr">
         <is>
-          <t>2025-03-24</t>
+          <t>2025-03-31</t>
         </is>
       </c>
     </row>
@@ -1526,7 +1523,6 @@
           <t>1.65</t>
         </is>
       </c>
-      <c r="C31" t="inlineStr"/>
       <c r="D31" t="inlineStr">
         <is>
           <t>Per 160 g</t>
@@ -1544,7 +1540,7 @@
       </c>
       <c r="G31" t="inlineStr">
         <is>
-          <t>2025-03-24</t>
+          <t>2025-03-31</t>
         </is>
       </c>
     </row>
@@ -1559,7 +1555,6 @@
           <t>1.65</t>
         </is>
       </c>
-      <c r="C32" t="inlineStr"/>
       <c r="D32" t="inlineStr">
         <is>
           <t>Per 160 g</t>
@@ -1577,7 +1572,7 @@
       </c>
       <c r="G32" t="inlineStr">
         <is>
-          <t>2025-03-24</t>
+          <t>2025-03-31</t>
         </is>
       </c>
     </row>
@@ -1592,7 +1587,6 @@
           <t>1.65</t>
         </is>
       </c>
-      <c r="C33" t="inlineStr"/>
       <c r="D33" t="inlineStr">
         <is>
           <t>Per 160 g</t>
@@ -1610,7 +1604,7 @@
       </c>
       <c r="G33" t="inlineStr">
         <is>
-          <t>2025-03-24</t>
+          <t>2025-03-31</t>
         </is>
       </c>
     </row>
@@ -1625,7 +1619,6 @@
           <t>1.49</t>
         </is>
       </c>
-      <c r="C34" t="inlineStr"/>
       <c r="D34" t="inlineStr">
         <is>
           <t>Per 200 g</t>
@@ -1643,7 +1636,7 @@
       </c>
       <c r="G34" t="inlineStr">
         <is>
-          <t>2025-03-24</t>
+          <t>2025-03-31</t>
         </is>
       </c>
     </row>
@@ -1658,7 +1651,6 @@
           <t>3.49</t>
         </is>
       </c>
-      <c r="C35" t="inlineStr"/>
       <c r="D35" t="inlineStr">
         <is>
           <t>Per 210 g</t>
@@ -1676,7 +1668,3419 @@
       </c>
       <c r="G35" t="inlineStr">
         <is>
-          <t>2025-03-24</t>
+          <t>2025-03-31</t>
+        </is>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="inlineStr">
+        <is>
+          <t>1 de Beste Choconino</t>
+        </is>
+      </c>
+      <c r="B36" t="inlineStr">
+        <is>
+          <t>1,79</t>
+        </is>
+      </c>
+      <c r="C36" t="inlineStr">
+        <is>
+          <t>Promo price not found</t>
+        </is>
+      </c>
+      <c r="D36" t="inlineStr">
+        <is>
+          <t>120 g</t>
+        </is>
+      </c>
+      <c r="E36" t="inlineStr">
+        <is>
+          <t>Non_Branded</t>
+        </is>
+      </c>
+      <c r="F36" t="inlineStr">
+        <is>
+          <t>Dirk</t>
+        </is>
+      </c>
+      <c r="G36" t="inlineStr">
+        <is>
+          <t>2025-03-31</t>
+        </is>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="inlineStr">
+        <is>
+          <t>1 de Beste Choco pinda's</t>
+        </is>
+      </c>
+      <c r="B37" t="inlineStr">
+        <is>
+          <t>1,55</t>
+        </is>
+      </c>
+      <c r="C37" t="inlineStr">
+        <is>
+          <t>Promo price not found</t>
+        </is>
+      </c>
+      <c r="D37" t="inlineStr">
+        <is>
+          <t>250 g</t>
+        </is>
+      </c>
+      <c r="E37" t="inlineStr">
+        <is>
+          <t>Non_Branded</t>
+        </is>
+      </c>
+      <c r="F37" t="inlineStr">
+        <is>
+          <t>Dirk</t>
+        </is>
+      </c>
+      <c r="G37" t="inlineStr">
+        <is>
+          <t>2025-03-31</t>
+        </is>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="inlineStr">
+        <is>
+          <t>1 de Beste Rozijnen chocolade</t>
+        </is>
+      </c>
+      <c r="B38" t="inlineStr">
+        <is>
+          <t>1,29</t>
+        </is>
+      </c>
+      <c r="C38" t="inlineStr">
+        <is>
+          <t>Promo price not found</t>
+        </is>
+      </c>
+      <c r="D38" t="inlineStr">
+        <is>
+          <t>200 g</t>
+        </is>
+      </c>
+      <c r="E38" t="inlineStr">
+        <is>
+          <t>Non_Branded</t>
+        </is>
+      </c>
+      <c r="F38" t="inlineStr">
+        <is>
+          <t>Dirk</t>
+        </is>
+      </c>
+      <c r="G38" t="inlineStr">
+        <is>
+          <t>2025-03-31</t>
+        </is>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="inlineStr">
+        <is>
+          <t>1 de Beste Choco crisp</t>
+        </is>
+      </c>
+      <c r="B39" t="inlineStr">
+        <is>
+          <t>2,19</t>
+        </is>
+      </c>
+      <c r="C39" t="inlineStr">
+        <is>
+          <t>Promo price not found</t>
+        </is>
+      </c>
+      <c r="D39" t="inlineStr">
+        <is>
+          <t>210 g</t>
+        </is>
+      </c>
+      <c r="E39" t="inlineStr">
+        <is>
+          <t>Non_Branded</t>
+        </is>
+      </c>
+      <c r="F39" t="inlineStr">
+        <is>
+          <t>Dirk</t>
+        </is>
+      </c>
+      <c r="G39" t="inlineStr">
+        <is>
+          <t>2025-03-31</t>
+        </is>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="inlineStr">
+        <is>
+          <t>1 de Beste Choco classic</t>
+        </is>
+      </c>
+      <c r="B40" t="inlineStr">
+        <is>
+          <t>1,75</t>
+        </is>
+      </c>
+      <c r="C40" t="inlineStr">
+        <is>
+          <t>Promo price not found</t>
+        </is>
+      </c>
+      <c r="D40" t="inlineStr">
+        <is>
+          <t>200 g</t>
+        </is>
+      </c>
+      <c r="E40" t="inlineStr">
+        <is>
+          <t>Non_Branded</t>
+        </is>
+      </c>
+      <c r="F40" t="inlineStr">
+        <is>
+          <t>Dirk</t>
+        </is>
+      </c>
+      <c r="G40" t="inlineStr">
+        <is>
+          <t>2025-03-31</t>
+        </is>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="inlineStr">
+        <is>
+          <t>1 de Beste Choco crunch</t>
+        </is>
+      </c>
+      <c r="B41" t="inlineStr">
+        <is>
+          <t>1,57</t>
+        </is>
+      </c>
+      <c r="C41" t="inlineStr">
+        <is>
+          <t>Promo price not found</t>
+        </is>
+      </c>
+      <c r="D41" t="inlineStr">
+        <is>
+          <t>150 g</t>
+        </is>
+      </c>
+      <c r="E41" t="inlineStr">
+        <is>
+          <t>Non_Branded</t>
+        </is>
+      </c>
+      <c r="F41" t="inlineStr">
+        <is>
+          <t>Dirk</t>
+        </is>
+      </c>
+      <c r="G41" t="inlineStr">
+        <is>
+          <t>2025-03-31</t>
+        </is>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="inlineStr">
+        <is>
+          <t>1 de Beste Choco pinda's</t>
+        </is>
+      </c>
+      <c r="B42" t="inlineStr">
+        <is>
+          <t>1,55</t>
+        </is>
+      </c>
+      <c r="C42" t="inlineStr">
+        <is>
+          <t>Promo price not found</t>
+        </is>
+      </c>
+      <c r="D42" t="inlineStr">
+        <is>
+          <t>250 g</t>
+        </is>
+      </c>
+      <c r="E42" t="inlineStr">
+        <is>
+          <t>Non_Branded</t>
+        </is>
+      </c>
+      <c r="F42" t="inlineStr">
+        <is>
+          <t>Dirk</t>
+        </is>
+      </c>
+      <c r="G42" t="inlineStr">
+        <is>
+          <t>2025-03-31</t>
+        </is>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="inlineStr">
+        <is>
+          <t>1 de Beste Chocolade pinda's</t>
+        </is>
+      </c>
+      <c r="B43" t="inlineStr">
+        <is>
+          <t>1,48</t>
+        </is>
+      </c>
+      <c r="C43" t="inlineStr">
+        <is>
+          <t>Promo price not found</t>
+        </is>
+      </c>
+      <c r="D43" t="inlineStr">
+        <is>
+          <t>200 g</t>
+        </is>
+      </c>
+      <c r="E43" t="inlineStr">
+        <is>
+          <t>Non_Branded</t>
+        </is>
+      </c>
+      <c r="F43" t="inlineStr">
+        <is>
+          <t>Dirk</t>
+        </is>
+      </c>
+      <c r="G43" t="inlineStr">
+        <is>
+          <t>2025-03-31</t>
+        </is>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="inlineStr">
+        <is>
+          <t>Lambertz Pindarotsjes melk</t>
+        </is>
+      </c>
+      <c r="B44" t="inlineStr">
+        <is>
+          <t>2,39</t>
+        </is>
+      </c>
+      <c r="C44" t="inlineStr">
+        <is>
+          <t>Promo price not found</t>
+        </is>
+      </c>
+      <c r="D44" t="inlineStr">
+        <is>
+          <t>250 g</t>
+        </is>
+      </c>
+      <c r="E44" t="inlineStr">
+        <is>
+          <t>Non_Branded</t>
+        </is>
+      </c>
+      <c r="F44" t="inlineStr">
+        <is>
+          <t>Dirk</t>
+        </is>
+      </c>
+      <c r="G44" t="inlineStr">
+        <is>
+          <t>2025-03-31</t>
+        </is>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="inlineStr">
+        <is>
+          <t>Chocolade cookie fudge rotsjes melk</t>
+        </is>
+      </c>
+      <c r="B45" t="inlineStr">
+        <is>
+          <t>2,49</t>
+        </is>
+      </c>
+      <c r="C45" t="inlineStr">
+        <is>
+          <t>Promo price not found</t>
+        </is>
+      </c>
+      <c r="D45" t="inlineStr">
+        <is>
+          <t>150 g</t>
+        </is>
+      </c>
+      <c r="E45" t="inlineStr">
+        <is>
+          <t>Non_Branded</t>
+        </is>
+      </c>
+      <c r="F45" t="inlineStr">
+        <is>
+          <t>Dirk</t>
+        </is>
+      </c>
+      <c r="G45" t="inlineStr">
+        <is>
+          <t>2025-03-31</t>
+        </is>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" t="inlineStr">
+        <is>
+          <t>1Bite Chocolade pindarotsjes puur</t>
+        </is>
+      </c>
+      <c r="B46" t="inlineStr">
+        <is>
+          <t>2,49</t>
+        </is>
+      </c>
+      <c r="C46" t="inlineStr">
+        <is>
+          <t>Promo price not found</t>
+        </is>
+      </c>
+      <c r="D46" t="inlineStr">
+        <is>
+          <t>150 g</t>
+        </is>
+      </c>
+      <c r="E46" t="inlineStr">
+        <is>
+          <t>Non_Branded</t>
+        </is>
+      </c>
+      <c r="F46" t="inlineStr">
+        <is>
+          <t>Dirk</t>
+        </is>
+      </c>
+      <c r="G46" t="inlineStr">
+        <is>
+          <t>2025-03-31</t>
+        </is>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" t="inlineStr">
+        <is>
+          <t>Ovaal drie chocolades 900 ml</t>
+        </is>
+      </c>
+      <c r="B47" t="inlineStr">
+        <is>
+          <t>2.99</t>
+        </is>
+      </c>
+      <c r="C47" t="inlineStr">
+        <is>
+          <t>Promo price not found</t>
+        </is>
+      </c>
+      <c r="D47" t="inlineStr">
+        <is>
+          <t>Weight not found</t>
+        </is>
+      </c>
+      <c r="E47" t="inlineStr">
+        <is>
+          <t>Non_Branded</t>
+        </is>
+      </c>
+      <c r="F47" t="inlineStr">
+        <is>
+          <t>Vomar</t>
+        </is>
+      </c>
+      <c r="G47" t="inlineStr">
+        <is>
+          <t>2025-03-31</t>
+        </is>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" t="inlineStr">
+        <is>
+          <t>G'woon choco classic</t>
+        </is>
+      </c>
+      <c r="B48" t="inlineStr">
+        <is>
+          <t>1.75</t>
+        </is>
+      </c>
+      <c r="C48" t="inlineStr">
+        <is>
+          <t>Promo price not found</t>
+        </is>
+      </c>
+      <c r="D48" t="inlineStr">
+        <is>
+          <t>Weight not found</t>
+        </is>
+      </c>
+      <c r="E48" t="inlineStr">
+        <is>
+          <t>Non_Branded</t>
+        </is>
+      </c>
+      <c r="F48" t="inlineStr">
+        <is>
+          <t>Vomar</t>
+        </is>
+      </c>
+      <c r="G48" t="inlineStr">
+        <is>
+          <t>2025-03-31</t>
+        </is>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" t="inlineStr">
+        <is>
+          <t>G'woon dip cookie choco 200gr</t>
+        </is>
+      </c>
+      <c r="B49" t="inlineStr">
+        <is>
+          <t>2.19</t>
+        </is>
+      </c>
+      <c r="C49" t="inlineStr">
+        <is>
+          <t>Promo price not found</t>
+        </is>
+      </c>
+      <c r="D49" t="inlineStr">
+        <is>
+          <t>Weight not found</t>
+        </is>
+      </c>
+      <c r="E49" t="inlineStr">
+        <is>
+          <t>Non_Branded</t>
+        </is>
+      </c>
+      <c r="F49" t="inlineStr">
+        <is>
+          <t>Vomar</t>
+        </is>
+      </c>
+      <c r="G49" t="inlineStr">
+        <is>
+          <t>2025-03-31</t>
+        </is>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" t="inlineStr">
+        <is>
+          <t>G'woon choco ruitjes</t>
+        </is>
+      </c>
+      <c r="B50" t="inlineStr">
+        <is>
+          <t>1.99</t>
+        </is>
+      </c>
+      <c r="C50" t="inlineStr">
+        <is>
+          <t>Promo price not found</t>
+        </is>
+      </c>
+      <c r="D50" t="inlineStr">
+        <is>
+          <t>Weight not found</t>
+        </is>
+      </c>
+      <c r="E50" t="inlineStr">
+        <is>
+          <t>Non_Branded</t>
+        </is>
+      </c>
+      <c r="F50" t="inlineStr">
+        <is>
+          <t>Vomar</t>
+        </is>
+      </c>
+      <c r="G50" t="inlineStr">
+        <is>
+          <t>2025-03-31</t>
+        </is>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" t="inlineStr">
+        <is>
+          <t>G'woon choco pinda 250gr</t>
+        </is>
+      </c>
+      <c r="B51" t="inlineStr">
+        <is>
+          <t>1.55</t>
+        </is>
+      </c>
+      <c r="C51" t="inlineStr">
+        <is>
+          <t>Promo price not found</t>
+        </is>
+      </c>
+      <c r="D51" t="inlineStr">
+        <is>
+          <t>Weight not found</t>
+        </is>
+      </c>
+      <c r="E51" t="inlineStr">
+        <is>
+          <t>Non_Branded</t>
+        </is>
+      </c>
+      <c r="F51" t="inlineStr">
+        <is>
+          <t>Vomar</t>
+        </is>
+      </c>
+      <c r="G51" t="inlineStr">
+        <is>
+          <t>2025-03-31</t>
+        </is>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" t="inlineStr">
+        <is>
+          <t>G'woon chocoprentjes melk</t>
+        </is>
+      </c>
+      <c r="B52" t="inlineStr">
+        <is>
+          <t>1.75</t>
+        </is>
+      </c>
+      <c r="C52" t="inlineStr">
+        <is>
+          <t>Promo price not found</t>
+        </is>
+      </c>
+      <c r="D52" t="inlineStr">
+        <is>
+          <t>Weight not found</t>
+        </is>
+      </c>
+      <c r="E52" t="inlineStr">
+        <is>
+          <t>Non_Branded</t>
+        </is>
+      </c>
+      <c r="F52" t="inlineStr">
+        <is>
+          <t>Vomar</t>
+        </is>
+      </c>
+      <c r="G52" t="inlineStr">
+        <is>
+          <t>2025-03-31</t>
+        </is>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" t="inlineStr">
+        <is>
+          <t>G'woon choco crunch 150gr</t>
+        </is>
+      </c>
+      <c r="B53" t="inlineStr">
+        <is>
+          <t>1.57</t>
+        </is>
+      </c>
+      <c r="C53" t="inlineStr">
+        <is>
+          <t>Promo price not found</t>
+        </is>
+      </c>
+      <c r="D53" t="inlineStr">
+        <is>
+          <t>Weight not found</t>
+        </is>
+      </c>
+      <c r="E53" t="inlineStr">
+        <is>
+          <t>Non_Branded</t>
+        </is>
+      </c>
+      <c r="F53" t="inlineStr">
+        <is>
+          <t>Vomar</t>
+        </is>
+      </c>
+      <c r="G53" t="inlineStr">
+        <is>
+          <t>2025-03-31</t>
+        </is>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" t="inlineStr">
+        <is>
+          <t>G'woon mini choco amandel 8st</t>
+        </is>
+      </c>
+      <c r="B54" t="inlineStr">
+        <is>
+          <t>2.49</t>
+        </is>
+      </c>
+      <c r="C54" t="inlineStr">
+        <is>
+          <t>Promo price not found</t>
+        </is>
+      </c>
+      <c r="D54" t="inlineStr">
+        <is>
+          <t>Weight not found</t>
+        </is>
+      </c>
+      <c r="E54" t="inlineStr">
+        <is>
+          <t>Non_Branded</t>
+        </is>
+      </c>
+      <c r="F54" t="inlineStr">
+        <is>
+          <t>Vomar</t>
+        </is>
+      </c>
+      <c r="G54" t="inlineStr">
+        <is>
+          <t>2025-03-31</t>
+        </is>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" t="inlineStr">
+        <is>
+          <t>G'woon biscuit duo choco 500gr</t>
+        </is>
+      </c>
+      <c r="B55" t="inlineStr">
+        <is>
+          <t>1.39</t>
+        </is>
+      </c>
+      <c r="C55" t="inlineStr">
+        <is>
+          <t>Promo price not found</t>
+        </is>
+      </c>
+      <c r="D55" t="inlineStr">
+        <is>
+          <t>Weight not found</t>
+        </is>
+      </c>
+      <c r="E55" t="inlineStr">
+        <is>
+          <t>Non_Branded</t>
+        </is>
+      </c>
+      <c r="F55" t="inlineStr">
+        <is>
+          <t>Vomar</t>
+        </is>
+      </c>
+      <c r="G55" t="inlineStr">
+        <is>
+          <t>2025-03-31</t>
+        </is>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" t="inlineStr">
+        <is>
+          <t>G'woon pindakoek melkchocolade</t>
+        </is>
+      </c>
+      <c r="B56" t="inlineStr">
+        <is>
+          <t>1.89</t>
+        </is>
+      </c>
+      <c r="C56" t="inlineStr">
+        <is>
+          <t>Promo price not found</t>
+        </is>
+      </c>
+      <c r="D56" t="inlineStr">
+        <is>
+          <t>Weight not found</t>
+        </is>
+      </c>
+      <c r="E56" t="inlineStr">
+        <is>
+          <t>Non_Branded</t>
+        </is>
+      </c>
+      <c r="F56" t="inlineStr">
+        <is>
+          <t>Vomar</t>
+        </is>
+      </c>
+      <c r="G56" t="inlineStr">
+        <is>
+          <t>2025-03-31</t>
+        </is>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" t="inlineStr">
+        <is>
+          <t>G'woon choco hazelnoot 200gr</t>
+        </is>
+      </c>
+      <c r="B57" t="inlineStr">
+        <is>
+          <t>1.94</t>
+        </is>
+      </c>
+      <c r="C57" t="inlineStr">
+        <is>
+          <t>Promo price not found</t>
+        </is>
+      </c>
+      <c r="D57" t="inlineStr">
+        <is>
+          <t>Weight not found</t>
+        </is>
+      </c>
+      <c r="E57" t="inlineStr">
+        <is>
+          <t>Non_Branded</t>
+        </is>
+      </c>
+      <c r="F57" t="inlineStr">
+        <is>
+          <t>Vomar</t>
+        </is>
+      </c>
+      <c r="G57" t="inlineStr">
+        <is>
+          <t>2025-03-31</t>
+        </is>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" t="inlineStr">
+        <is>
+          <t>G'woon melkbiscuit choco</t>
+        </is>
+      </c>
+      <c r="B58" t="inlineStr">
+        <is>
+          <t>1.49</t>
+        </is>
+      </c>
+      <c r="C58" t="inlineStr">
+        <is>
+          <t>Promo price not found</t>
+        </is>
+      </c>
+      <c r="D58" t="inlineStr">
+        <is>
+          <t>Weight not found</t>
+        </is>
+      </c>
+      <c r="E58" t="inlineStr">
+        <is>
+          <t>Non_Branded</t>
+        </is>
+      </c>
+      <c r="F58" t="inlineStr">
+        <is>
+          <t>Vomar</t>
+        </is>
+      </c>
+      <c r="G58" t="inlineStr">
+        <is>
+          <t>2025-03-31</t>
+        </is>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" t="inlineStr">
+        <is>
+          <t>G'woon choco rozijnen 200 gr</t>
+        </is>
+      </c>
+      <c r="B59" t="inlineStr">
+        <is>
+          <t>1.49</t>
+        </is>
+      </c>
+      <c r="C59" t="inlineStr">
+        <is>
+          <t>Promo price not found</t>
+        </is>
+      </c>
+      <c r="D59" t="inlineStr">
+        <is>
+          <t>Weight not found</t>
+        </is>
+      </c>
+      <c r="E59" t="inlineStr">
+        <is>
+          <t>Non_Branded</t>
+        </is>
+      </c>
+      <c r="F59" t="inlineStr">
+        <is>
+          <t>Vomar</t>
+        </is>
+      </c>
+      <c r="G59" t="inlineStr">
+        <is>
+          <t>2025-03-31</t>
+        </is>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" t="inlineStr">
+        <is>
+          <t>G'woon choco crisp 210 gr</t>
+        </is>
+      </c>
+      <c r="B60" t="inlineStr">
+        <is>
+          <t>2.19</t>
+        </is>
+      </c>
+      <c r="C60" t="inlineStr">
+        <is>
+          <t>Promo price not found</t>
+        </is>
+      </c>
+      <c r="D60" t="inlineStr">
+        <is>
+          <t>Weight not found</t>
+        </is>
+      </c>
+      <c r="E60" t="inlineStr">
+        <is>
+          <t>Non_Branded</t>
+        </is>
+      </c>
+      <c r="F60" t="inlineStr">
+        <is>
+          <t>Vomar</t>
+        </is>
+      </c>
+      <c r="G60" t="inlineStr">
+        <is>
+          <t>2025-03-31</t>
+        </is>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" t="inlineStr">
+        <is>
+          <t>G'woon mini choco mix 12st</t>
+        </is>
+      </c>
+      <c r="B61" t="inlineStr">
+        <is>
+          <t>3.19</t>
+        </is>
+      </c>
+      <c r="C61" t="inlineStr">
+        <is>
+          <t>Promo price not found</t>
+        </is>
+      </c>
+      <c r="D61" t="inlineStr">
+        <is>
+          <t>Weight not found</t>
+        </is>
+      </c>
+      <c r="E61" t="inlineStr">
+        <is>
+          <t>Non_Branded</t>
+        </is>
+      </c>
+      <c r="F61" t="inlineStr">
+        <is>
+          <t>Vomar</t>
+        </is>
+      </c>
+      <c r="G61" t="inlineStr">
+        <is>
+          <t>2025-03-31</t>
+        </is>
+      </c>
+    </row>
+    <row r="62">
+      <c r="A62" t="inlineStr">
+        <is>
+          <t>G'woon granenbiscuit choco 292gr</t>
+        </is>
+      </c>
+      <c r="B62" t="inlineStr">
+        <is>
+          <t>1.89</t>
+        </is>
+      </c>
+      <c r="C62" t="inlineStr">
+        <is>
+          <t>Promo price not found</t>
+        </is>
+      </c>
+      <c r="D62" t="inlineStr">
+        <is>
+          <t>Weight not found</t>
+        </is>
+      </c>
+      <c r="E62" t="inlineStr">
+        <is>
+          <t>Non_Branded</t>
+        </is>
+      </c>
+      <c r="F62" t="inlineStr">
+        <is>
+          <t>Vomar</t>
+        </is>
+      </c>
+      <c r="G62" t="inlineStr">
+        <is>
+          <t>2025-03-31</t>
+        </is>
+      </c>
+    </row>
+    <row r="63">
+      <c r="A63" t="inlineStr">
+        <is>
+          <t>G'woon chocosticks vanille 12</t>
+        </is>
+      </c>
+      <c r="B63" t="inlineStr">
+        <is>
+          <t>1.89</t>
+        </is>
+      </c>
+      <c r="C63" t="inlineStr">
+        <is>
+          <t>Promo price not found</t>
+        </is>
+      </c>
+      <c r="D63" t="inlineStr">
+        <is>
+          <t>Weight not found</t>
+        </is>
+      </c>
+      <c r="E63" t="inlineStr">
+        <is>
+          <t>Non_Branded</t>
+        </is>
+      </c>
+      <c r="F63" t="inlineStr">
+        <is>
+          <t>Vomar</t>
+        </is>
+      </c>
+      <c r="G63" t="inlineStr">
+        <is>
+          <t>2025-03-31</t>
+        </is>
+      </c>
+    </row>
+    <row r="64">
+      <c r="A64" t="inlineStr">
+        <is>
+          <t>G'woon chocoprentjes puur</t>
+        </is>
+      </c>
+      <c r="B64" t="inlineStr">
+        <is>
+          <t>1.75</t>
+        </is>
+      </c>
+      <c r="C64" t="inlineStr">
+        <is>
+          <t>Promo price not found</t>
+        </is>
+      </c>
+      <c r="D64" t="inlineStr">
+        <is>
+          <t>Weight not found</t>
+        </is>
+      </c>
+      <c r="E64" t="inlineStr">
+        <is>
+          <t>Non_Branded</t>
+        </is>
+      </c>
+      <c r="F64" t="inlineStr">
+        <is>
+          <t>Vomar</t>
+        </is>
+      </c>
+      <c r="G64" t="inlineStr">
+        <is>
+          <t>2025-03-31</t>
+        </is>
+      </c>
+    </row>
+    <row r="65">
+      <c r="A65" t="inlineStr">
+        <is>
+          <t>G'woon choconino 5 stuks</t>
+        </is>
+      </c>
+      <c r="B65" t="inlineStr">
+        <is>
+          <t>1.89</t>
+        </is>
+      </c>
+      <c r="C65" t="inlineStr">
+        <is>
+          <t>Promo price not found</t>
+        </is>
+      </c>
+      <c r="D65" t="inlineStr">
+        <is>
+          <t>Weight not found</t>
+        </is>
+      </c>
+      <c r="E65" t="inlineStr">
+        <is>
+          <t>Non_Branded</t>
+        </is>
+      </c>
+      <c r="F65" t="inlineStr">
+        <is>
+          <t>Vomar</t>
+        </is>
+      </c>
+      <c r="G65" t="inlineStr">
+        <is>
+          <t>2025-03-31</t>
+        </is>
+      </c>
+    </row>
+    <row r="66">
+      <c r="A66" t="inlineStr">
+        <is>
+          <t>G'woon mega choco's amandel 6s</t>
+        </is>
+      </c>
+      <c r="B66" t="inlineStr">
+        <is>
+          <t>3.79</t>
+        </is>
+      </c>
+      <c r="C66" t="inlineStr">
+        <is>
+          <t>Promo price not found</t>
+        </is>
+      </c>
+      <c r="D66" t="inlineStr">
+        <is>
+          <t>Weight not found</t>
+        </is>
+      </c>
+      <c r="E66" t="inlineStr">
+        <is>
+          <t>Non_Branded</t>
+        </is>
+      </c>
+      <c r="F66" t="inlineStr">
+        <is>
+          <t>Vomar</t>
+        </is>
+      </c>
+      <c r="G66" t="inlineStr">
+        <is>
+          <t>2025-03-31</t>
+        </is>
+      </c>
+    </row>
+    <row r="67">
+      <c r="A67" t="inlineStr">
+        <is>
+          <t>G'woon mega choco's wit 6st</t>
+        </is>
+      </c>
+      <c r="B67" t="inlineStr">
+        <is>
+          <t>3.79</t>
+        </is>
+      </c>
+      <c r="C67" t="inlineStr">
+        <is>
+          <t>Promo price not found</t>
+        </is>
+      </c>
+      <c r="D67" t="inlineStr">
+        <is>
+          <t>Weight not found</t>
+        </is>
+      </c>
+      <c r="E67" t="inlineStr">
+        <is>
+          <t>Non_Branded</t>
+        </is>
+      </c>
+      <c r="F67" t="inlineStr">
+        <is>
+          <t>Vomar</t>
+        </is>
+      </c>
+      <c r="G67" t="inlineStr">
+        <is>
+          <t>2025-03-31</t>
+        </is>
+      </c>
+    </row>
+    <row r="68">
+      <c r="A68" t="inlineStr">
+        <is>
+          <t>G'woon mega choco's melk 6st</t>
+        </is>
+      </c>
+      <c r="B68" t="inlineStr">
+        <is>
+          <t>3.79</t>
+        </is>
+      </c>
+      <c r="C68" t="inlineStr">
+        <is>
+          <t>Promo price not found</t>
+        </is>
+      </c>
+      <c r="D68" t="inlineStr">
+        <is>
+          <t>Weight not found</t>
+        </is>
+      </c>
+      <c r="E68" t="inlineStr">
+        <is>
+          <t>Non_Branded</t>
+        </is>
+      </c>
+      <c r="F68" t="inlineStr">
+        <is>
+          <t>Vomar</t>
+        </is>
+      </c>
+      <c r="G68" t="inlineStr">
+        <is>
+          <t>2025-03-31</t>
+        </is>
+      </c>
+    </row>
+    <row r="69">
+      <c r="A69" t="inlineStr">
+        <is>
+          <t>Pindarotsjes</t>
+        </is>
+      </c>
+      <c r="B69" t="inlineStr">
+        <is>
+          <t>2.39</t>
+        </is>
+      </c>
+      <c r="C69" t="inlineStr">
+        <is>
+          <t>No promo price</t>
+        </is>
+      </c>
+      <c r="D69" t="inlineStr">
+        <is>
+          <t>250 g</t>
+        </is>
+      </c>
+      <c r="E69" t="inlineStr">
+        <is>
+          <t>Non_Branded</t>
+        </is>
+      </c>
+      <c r="F69" t="inlineStr">
+        <is>
+          <t>Aldi</t>
+        </is>
+      </c>
+      <c r="G69" t="inlineStr">
+        <is>
+          <t>2025-03-31</t>
+        </is>
+      </c>
+    </row>
+    <row r="70">
+      <c r="A70" t="inlineStr">
+        <is>
+          <t>Air power</t>
+        </is>
+      </c>
+      <c r="B70" t="inlineStr">
+        <is>
+          <t>1.89</t>
+        </is>
+      </c>
+      <c r="C70" t="inlineStr">
+        <is>
+          <t>No promo price</t>
+        </is>
+      </c>
+      <c r="D70" t="inlineStr">
+        <is>
+          <t>150 g</t>
+        </is>
+      </c>
+      <c r="E70" t="inlineStr">
+        <is>
+          <t>Non_Branded</t>
+        </is>
+      </c>
+      <c r="F70" t="inlineStr">
+        <is>
+          <t>Aldi</t>
+        </is>
+      </c>
+      <c r="G70" t="inlineStr">
+        <is>
+          <t>2025-03-31</t>
+        </is>
+      </c>
+    </row>
+    <row r="71">
+      <c r="A71" t="inlineStr">
+        <is>
+          <t>Candy bars</t>
+        </is>
+      </c>
+      <c r="B71" t="inlineStr">
+        <is>
+          <t>2.19</t>
+        </is>
+      </c>
+      <c r="C71" t="inlineStr">
+        <is>
+          <t>No promo price</t>
+        </is>
+      </c>
+      <c r="D71" t="inlineStr">
+        <is>
+          <t>6x50 g</t>
+        </is>
+      </c>
+      <c r="E71" t="inlineStr">
+        <is>
+          <t>Non_Branded</t>
+        </is>
+      </c>
+      <c r="F71" t="inlineStr">
+        <is>
+          <t>Aldi</t>
+        </is>
+      </c>
+      <c r="G71" t="inlineStr">
+        <is>
+          <t>2025-03-31</t>
+        </is>
+      </c>
+    </row>
+    <row r="72">
+      <c r="A72" t="inlineStr">
+        <is>
+          <t>Melkchocolade pinda's</t>
+        </is>
+      </c>
+      <c r="B72" t="inlineStr">
+        <is>
+          <t>1.79</t>
+        </is>
+      </c>
+      <c r="C72" t="inlineStr">
+        <is>
+          <t>No promo price</t>
+        </is>
+      </c>
+      <c r="D72" t="inlineStr">
+        <is>
+          <t>200 g</t>
+        </is>
+      </c>
+      <c r="E72" t="inlineStr">
+        <is>
+          <t>Non_Branded</t>
+        </is>
+      </c>
+      <c r="F72" t="inlineStr">
+        <is>
+          <t>Aldi</t>
+        </is>
+      </c>
+      <c r="G72" t="inlineStr">
+        <is>
+          <t>2025-03-31</t>
+        </is>
+      </c>
+    </row>
+    <row r="73">
+      <c r="A73" t="inlineStr">
+        <is>
+          <t>Chocolade pindakoeken</t>
+        </is>
+      </c>
+      <c r="B73" t="inlineStr">
+        <is>
+          <t>1.99</t>
+        </is>
+      </c>
+      <c r="C73" t="inlineStr">
+        <is>
+          <t>No promo price</t>
+        </is>
+      </c>
+      <c r="D73" t="inlineStr">
+        <is>
+          <t>Inhoud: 6 stuks, 200 g</t>
+        </is>
+      </c>
+      <c r="E73" t="inlineStr">
+        <is>
+          <t>Non_Branded</t>
+        </is>
+      </c>
+      <c r="F73" t="inlineStr">
+        <is>
+          <t>Aldi</t>
+        </is>
+      </c>
+      <c r="G73" t="inlineStr">
+        <is>
+          <t>2025-03-31</t>
+        </is>
+      </c>
+    </row>
+    <row r="74">
+      <c r="A74" t="inlineStr">
+        <is>
+          <t>Pindarotsjes</t>
+        </is>
+      </c>
+      <c r="B74" t="inlineStr">
+        <is>
+          <t>2.39</t>
+        </is>
+      </c>
+      <c r="C74" t="inlineStr">
+        <is>
+          <t>No promo price</t>
+        </is>
+      </c>
+      <c r="D74" t="inlineStr">
+        <is>
+          <t>250 g</t>
+        </is>
+      </c>
+      <c r="E74" t="inlineStr">
+        <is>
+          <t>Non_Branded</t>
+        </is>
+      </c>
+      <c r="F74" t="inlineStr">
+        <is>
+          <t>Aldi</t>
+        </is>
+      </c>
+      <c r="G74" t="inlineStr">
+        <is>
+          <t>2025-03-31</t>
+        </is>
+      </c>
+    </row>
+    <row r="75">
+      <c r="A75" t="inlineStr">
+        <is>
+          <t>M&amp;M'S Melk chocolade pinda snoepjes maxi</t>
+        </is>
+      </c>
+      <c r="B75" t="inlineStr">
+        <is>
+          <t>Promo price not found</t>
+        </is>
+      </c>
+      <c r="C75" t="inlineStr">
+        <is>
+          <t>5,16</t>
+        </is>
+      </c>
+      <c r="D75" t="inlineStr">
+        <is>
+          <t>400 g</t>
+        </is>
+      </c>
+      <c r="E75" t="inlineStr">
+        <is>
+          <t>branded</t>
+        </is>
+      </c>
+      <c r="F75" t="inlineStr">
+        <is>
+          <t>Jumbo</t>
+        </is>
+      </c>
+      <c r="G75" t="inlineStr">
+        <is>
+          <t>2025-03-31</t>
+        </is>
+      </c>
+    </row>
+    <row r="76">
+      <c r="A76" t="inlineStr">
+        <is>
+          <t>M&amp;M'S Melk Chocolade Crispy Snoepjes Zak Groot</t>
+        </is>
+      </c>
+      <c r="B76" t="inlineStr">
+        <is>
+          <t>Promo price not found</t>
+        </is>
+      </c>
+      <c r="C76" t="inlineStr">
+        <is>
+          <t>5,54</t>
+        </is>
+      </c>
+      <c r="D76" t="inlineStr">
+        <is>
+          <t>340 g</t>
+        </is>
+      </c>
+      <c r="E76" t="inlineStr">
+        <is>
+          <t>branded</t>
+        </is>
+      </c>
+      <c r="F76" t="inlineStr">
+        <is>
+          <t>Jumbo</t>
+        </is>
+      </c>
+      <c r="G76" t="inlineStr">
+        <is>
+          <t>2025-03-31</t>
+        </is>
+      </c>
+    </row>
+    <row r="77">
+      <c r="A77" t="inlineStr">
+        <is>
+          <t>M&amp;M'S Choco melk chocolade snoepjes maxi</t>
+        </is>
+      </c>
+      <c r="B77" t="inlineStr">
+        <is>
+          <t>Promo price not found</t>
+        </is>
+      </c>
+      <c r="C77" t="inlineStr">
+        <is>
+          <t>5,12</t>
+        </is>
+      </c>
+      <c r="D77" t="inlineStr">
+        <is>
+          <t>400 g</t>
+        </is>
+      </c>
+      <c r="E77" t="inlineStr">
+        <is>
+          <t>branded</t>
+        </is>
+      </c>
+      <c r="F77" t="inlineStr">
+        <is>
+          <t>Jumbo</t>
+        </is>
+      </c>
+      <c r="G77" t="inlineStr">
+        <is>
+          <t>2025-03-31</t>
+        </is>
+      </c>
+    </row>
+    <row r="78">
+      <c r="A78" t="inlineStr">
+        <is>
+          <t>M&amp;M's Peanut 125 g</t>
+        </is>
+      </c>
+      <c r="B78" t="inlineStr">
+        <is>
+          <t>Promo price not found</t>
+        </is>
+      </c>
+      <c r="C78" t="inlineStr">
+        <is>
+          <t>2,08</t>
+        </is>
+      </c>
+      <c r="D78" t="inlineStr">
+        <is>
+          <t>125 g</t>
+        </is>
+      </c>
+      <c r="E78" t="inlineStr">
+        <is>
+          <t>branded</t>
+        </is>
+      </c>
+      <c r="F78" t="inlineStr">
+        <is>
+          <t>Jumbo</t>
+        </is>
+      </c>
+      <c r="G78" t="inlineStr">
+        <is>
+          <t>2025-03-31</t>
+        </is>
+      </c>
+    </row>
+    <row r="79">
+      <c r="A79" t="inlineStr">
+        <is>
+          <t>M&amp;M'S Melk Chocolade Crispy Snoepjes Zak Middel</t>
+        </is>
+      </c>
+      <c r="B79" t="inlineStr">
+        <is>
+          <t>Promo price not found</t>
+        </is>
+      </c>
+      <c r="C79" t="inlineStr">
+        <is>
+          <t>3,09</t>
+        </is>
+      </c>
+      <c r="D79" t="inlineStr">
+        <is>
+          <t>187 g</t>
+        </is>
+      </c>
+      <c r="E79" t="inlineStr">
+        <is>
+          <t>branded</t>
+        </is>
+      </c>
+      <c r="F79" t="inlineStr">
+        <is>
+          <t>Jumbo</t>
+        </is>
+      </c>
+      <c r="G79" t="inlineStr">
+        <is>
+          <t>2025-03-31</t>
+        </is>
+      </c>
+    </row>
+    <row r="80">
+      <c r="A80" t="inlineStr">
+        <is>
+          <t>M&amp;M'S Melk Chocolade Choco Snoepjes Zak Middel</t>
+        </is>
+      </c>
+      <c r="B80" t="inlineStr">
+        <is>
+          <t>Promo price not found</t>
+        </is>
+      </c>
+      <c r="C80" t="inlineStr">
+        <is>
+          <t>3,08</t>
+        </is>
+      </c>
+      <c r="D80" t="inlineStr">
+        <is>
+          <t>200 g</t>
+        </is>
+      </c>
+      <c r="E80" t="inlineStr">
+        <is>
+          <t>branded</t>
+        </is>
+      </c>
+      <c r="F80" t="inlineStr">
+        <is>
+          <t>Jumbo</t>
+        </is>
+      </c>
+      <c r="G80" t="inlineStr">
+        <is>
+          <t>2025-03-31</t>
+        </is>
+      </c>
+    </row>
+    <row r="81">
+      <c r="A81" t="inlineStr">
+        <is>
+          <t>M&amp;M'S Melk Chocolade Pinda Snoepjes Zak Middel</t>
+        </is>
+      </c>
+      <c r="B81" t="inlineStr">
+        <is>
+          <t>Promo price not found</t>
+        </is>
+      </c>
+      <c r="C81" t="inlineStr">
+        <is>
+          <t>3,09</t>
+        </is>
+      </c>
+      <c r="D81" t="inlineStr">
+        <is>
+          <t>200 g</t>
+        </is>
+      </c>
+      <c r="E81" t="inlineStr">
+        <is>
+          <t>branded</t>
+        </is>
+      </c>
+      <c r="F81" t="inlineStr">
+        <is>
+          <t>Jumbo</t>
+        </is>
+      </c>
+      <c r="G81" t="inlineStr">
+        <is>
+          <t>2025-03-31</t>
+        </is>
+      </c>
+    </row>
+    <row r="82">
+      <c r="A82" t="inlineStr">
+        <is>
+          <t>M&amp;M'S Minis melk chocolade choco snoepjes 176g</t>
+        </is>
+      </c>
+      <c r="B82" t="inlineStr">
+        <is>
+          <t>Promo price not found</t>
+        </is>
+      </c>
+      <c r="C82" t="inlineStr">
+        <is>
+          <t>3,36</t>
+        </is>
+      </c>
+      <c r="D82" t="inlineStr">
+        <is>
+          <t>176 g</t>
+        </is>
+      </c>
+      <c r="E82" t="inlineStr">
+        <is>
+          <t>branded</t>
+        </is>
+      </c>
+      <c r="F82" t="inlineStr">
+        <is>
+          <t>Jumbo</t>
+        </is>
+      </c>
+      <c r="G82" t="inlineStr">
+        <is>
+          <t>2025-03-31</t>
+        </is>
+      </c>
+    </row>
+    <row r="83">
+      <c r="A83" t="inlineStr">
+        <is>
+          <t>M&amp;M'S Melk Chocolade Crispy Snoepjes Zak Klein</t>
+        </is>
+      </c>
+      <c r="B83" t="inlineStr">
+        <is>
+          <t>Promo price not found</t>
+        </is>
+      </c>
+      <c r="C83" t="inlineStr">
+        <is>
+          <t>2,29</t>
+        </is>
+      </c>
+      <c r="D83" t="inlineStr">
+        <is>
+          <t>107 g</t>
+        </is>
+      </c>
+      <c r="E83" t="inlineStr">
+        <is>
+          <t>branded</t>
+        </is>
+      </c>
+      <c r="F83" t="inlineStr">
+        <is>
+          <t>Jumbo</t>
+        </is>
+      </c>
+      <c r="G83" t="inlineStr">
+        <is>
+          <t>2025-03-31</t>
+        </is>
+      </c>
+    </row>
+    <row r="84">
+      <c r="A84" t="inlineStr">
+        <is>
+          <t>M&amp;M'S Melk Chocolade Choco Snoepjes Zak Klein</t>
+        </is>
+      </c>
+      <c r="B84" t="inlineStr">
+        <is>
+          <t>Promo price not found</t>
+        </is>
+      </c>
+      <c r="C84" t="inlineStr">
+        <is>
+          <t>2,08</t>
+        </is>
+      </c>
+      <c r="D84" t="inlineStr">
+        <is>
+          <t>125 g</t>
+        </is>
+      </c>
+      <c r="E84" t="inlineStr">
+        <is>
+          <t>branded</t>
+        </is>
+      </c>
+      <c r="F84" t="inlineStr">
+        <is>
+          <t>Jumbo</t>
+        </is>
+      </c>
+      <c r="G84" t="inlineStr">
+        <is>
+          <t>2025-03-31</t>
+        </is>
+      </c>
+    </row>
+    <row r="85">
+      <c r="A85" t="inlineStr">
+        <is>
+          <t>M&amp;M's Mini Cookie 180g</t>
+        </is>
+      </c>
+      <c r="B85" t="inlineStr">
+        <is>
+          <t>Promo price not found</t>
+        </is>
+      </c>
+      <c r="C85" t="inlineStr">
+        <is>
+          <t>2,69</t>
+        </is>
+      </c>
+      <c r="D85" t="inlineStr">
+        <is>
+          <t>Weight not found</t>
+        </is>
+      </c>
+      <c r="E85" t="inlineStr">
+        <is>
+          <t>branded</t>
+        </is>
+      </c>
+      <c r="F85" t="inlineStr">
+        <is>
+          <t>Jumbo</t>
+        </is>
+      </c>
+      <c r="G85" t="inlineStr">
+        <is>
+          <t>2025-03-31</t>
+        </is>
+      </c>
+    </row>
+    <row r="86">
+      <c r="A86" t="inlineStr">
+        <is>
+          <t>M&amp;M'S Melk Chocolade Gezouten Karamel Snoepjes Zak Middel</t>
+        </is>
+      </c>
+      <c r="B86" t="inlineStr">
+        <is>
+          <t>Promo price not found</t>
+        </is>
+      </c>
+      <c r="C86" t="inlineStr">
+        <is>
+          <t>2,68</t>
+        </is>
+      </c>
+      <c r="D86" t="inlineStr">
+        <is>
+          <t>176 g</t>
+        </is>
+      </c>
+      <c r="E86" t="inlineStr">
+        <is>
+          <t>branded</t>
+        </is>
+      </c>
+      <c r="F86" t="inlineStr">
+        <is>
+          <t>Jumbo</t>
+        </is>
+      </c>
+      <c r="G86" t="inlineStr">
+        <is>
+          <t>2025-03-31</t>
+        </is>
+      </c>
+    </row>
+    <row r="87">
+      <c r="A87" t="inlineStr">
+        <is>
+          <t>M&amp;M'S Melk chocolade gezouten karamel snoepjes maxi</t>
+        </is>
+      </c>
+      <c r="B87" t="inlineStr">
+        <is>
+          <t>Promo price not found</t>
+        </is>
+      </c>
+      <c r="C87" t="inlineStr">
+        <is>
+          <t>5,53</t>
+        </is>
+      </c>
+      <c r="D87" t="inlineStr">
+        <is>
+          <t>367 g</t>
+        </is>
+      </c>
+      <c r="E87" t="inlineStr">
+        <is>
+          <t>branded</t>
+        </is>
+      </c>
+      <c r="F87" t="inlineStr">
+        <is>
+          <t>Jumbo</t>
+        </is>
+      </c>
+      <c r="G87" t="inlineStr">
+        <is>
+          <t>2025-03-31</t>
+        </is>
+      </c>
+    </row>
+    <row r="88">
+      <c r="A88" t="inlineStr">
+        <is>
+          <t>M&amp;M'S Melk chocolade pinda snoepjes</t>
+        </is>
+      </c>
+      <c r="B88" t="inlineStr">
+        <is>
+          <t>5.39</t>
+        </is>
+      </c>
+      <c r="C88" t="inlineStr"/>
+      <c r="D88" t="inlineStr">
+        <is>
+          <t>Per 400 g</t>
+        </is>
+      </c>
+      <c r="E88" t="inlineStr">
+        <is>
+          <t>branded</t>
+        </is>
+      </c>
+      <c r="F88" t="inlineStr">
+        <is>
+          <t>Plus</t>
+        </is>
+      </c>
+      <c r="G88" t="inlineStr">
+        <is>
+          <t>2025-03-31</t>
+        </is>
+      </c>
+    </row>
+    <row r="89">
+      <c r="A89" t="inlineStr">
+        <is>
+          <t>M&amp;M'S Minis chocolade snoepjes maxi</t>
+        </is>
+      </c>
+      <c r="B89" t="inlineStr">
+        <is>
+          <t>5.49</t>
+        </is>
+      </c>
+      <c r="C89" t="inlineStr"/>
+      <c r="D89" t="inlineStr">
+        <is>
+          <t>Per 360 g</t>
+        </is>
+      </c>
+      <c r="E89" t="inlineStr">
+        <is>
+          <t>branded</t>
+        </is>
+      </c>
+      <c r="F89" t="inlineStr">
+        <is>
+          <t>Plus</t>
+        </is>
+      </c>
+      <c r="G89" t="inlineStr">
+        <is>
+          <t>2025-03-31</t>
+        </is>
+      </c>
+    </row>
+    <row r="90">
+      <c r="A90" t="inlineStr">
+        <is>
+          <t>M&amp;M'S Pinda chocolade snoepjes zak</t>
+        </is>
+      </c>
+      <c r="B90" t="inlineStr">
+        <is>
+          <t>3.39</t>
+        </is>
+      </c>
+      <c r="C90" t="inlineStr"/>
+      <c r="D90" t="inlineStr">
+        <is>
+          <t>Per 200 g</t>
+        </is>
+      </c>
+      <c r="E90" t="inlineStr">
+        <is>
+          <t>branded</t>
+        </is>
+      </c>
+      <c r="F90" t="inlineStr">
+        <is>
+          <t>Plus</t>
+        </is>
+      </c>
+      <c r="G90" t="inlineStr">
+        <is>
+          <t>2025-03-31</t>
+        </is>
+      </c>
+    </row>
+    <row r="91">
+      <c r="A91" t="inlineStr">
+        <is>
+          <t>M&amp;M'S Melk chocolade karamel snoepjes</t>
+        </is>
+      </c>
+      <c r="B91" t="inlineStr">
+        <is>
+          <t>5.49</t>
+        </is>
+      </c>
+      <c r="C91" t="inlineStr"/>
+      <c r="D91" t="inlineStr">
+        <is>
+          <t>Per 367 g</t>
+        </is>
+      </c>
+      <c r="E91" t="inlineStr">
+        <is>
+          <t>branded</t>
+        </is>
+      </c>
+      <c r="F91" t="inlineStr">
+        <is>
+          <t>Plus</t>
+        </is>
+      </c>
+      <c r="G91" t="inlineStr">
+        <is>
+          <t>2025-03-31</t>
+        </is>
+      </c>
+    </row>
+    <row r="92">
+      <c r="A92" t="inlineStr">
+        <is>
+          <t>M&amp;M'S Melk chocolade choco snoepjes zak</t>
+        </is>
+      </c>
+      <c r="B92" t="inlineStr">
+        <is>
+          <t>5.39</t>
+        </is>
+      </c>
+      <c r="C92" t="inlineStr"/>
+      <c r="D92" t="inlineStr">
+        <is>
+          <t>Per 400 g</t>
+        </is>
+      </c>
+      <c r="E92" t="inlineStr">
+        <is>
+          <t>branded</t>
+        </is>
+      </c>
+      <c r="F92" t="inlineStr">
+        <is>
+          <t>Plus</t>
+        </is>
+      </c>
+      <c r="G92" t="inlineStr">
+        <is>
+          <t>2025-03-31</t>
+        </is>
+      </c>
+    </row>
+    <row r="93">
+      <c r="A93" t="inlineStr">
+        <is>
+          <t>M&amp;M'S Melk Chocolade Crispy</t>
+        </is>
+      </c>
+      <c r="B93" t="inlineStr">
+        <is>
+          <t>5.39</t>
+        </is>
+      </c>
+      <c r="C93" t="inlineStr"/>
+      <c r="D93" t="inlineStr">
+        <is>
+          <t>Per 340 g</t>
+        </is>
+      </c>
+      <c r="E93" t="inlineStr">
+        <is>
+          <t>branded</t>
+        </is>
+      </c>
+      <c r="F93" t="inlineStr">
+        <is>
+          <t>Plus</t>
+        </is>
+      </c>
+      <c r="G93" t="inlineStr">
+        <is>
+          <t>2025-03-31</t>
+        </is>
+      </c>
+    </row>
+    <row r="94">
+      <c r="A94" t="inlineStr">
+        <is>
+          <t xml:space="preserve">M&amp;M'S Melk Chocolade Choco </t>
+        </is>
+      </c>
+      <c r="B94" t="inlineStr">
+        <is>
+          <t>3.39</t>
+        </is>
+      </c>
+      <c r="C94" t="inlineStr"/>
+      <c r="D94" t="inlineStr">
+        <is>
+          <t>Per 200 g</t>
+        </is>
+      </c>
+      <c r="E94" t="inlineStr">
+        <is>
+          <t>branded</t>
+        </is>
+      </c>
+      <c r="F94" t="inlineStr">
+        <is>
+          <t>Plus</t>
+        </is>
+      </c>
+      <c r="G94" t="inlineStr">
+        <is>
+          <t>2025-03-31</t>
+        </is>
+      </c>
+    </row>
+    <row r="95">
+      <c r="A95" t="inlineStr">
+        <is>
+          <t xml:space="preserve">M&amp;M'S Melk Chocolade Crispy </t>
+        </is>
+      </c>
+      <c r="B95" t="inlineStr">
+        <is>
+          <t>3.39</t>
+        </is>
+      </c>
+      <c r="C95" t="inlineStr"/>
+      <c r="D95" t="inlineStr">
+        <is>
+          <t>Per 187 g</t>
+        </is>
+      </c>
+      <c r="E95" t="inlineStr">
+        <is>
+          <t>branded</t>
+        </is>
+      </c>
+      <c r="F95" t="inlineStr">
+        <is>
+          <t>Plus</t>
+        </is>
+      </c>
+      <c r="G95" t="inlineStr">
+        <is>
+          <t>2025-03-31</t>
+        </is>
+      </c>
+    </row>
+    <row r="96">
+      <c r="A96" t="inlineStr">
+        <is>
+          <t>M&amp;M'S Melk Chocolade Salted Caramel</t>
+        </is>
+      </c>
+      <c r="B96" t="inlineStr">
+        <is>
+          <t>2.95</t>
+        </is>
+      </c>
+      <c r="C96" t="inlineStr"/>
+      <c r="D96" t="inlineStr">
+        <is>
+          <t>Per 176 g</t>
+        </is>
+      </c>
+      <c r="E96" t="inlineStr">
+        <is>
+          <t>branded</t>
+        </is>
+      </c>
+      <c r="F96" t="inlineStr">
+        <is>
+          <t>Plus</t>
+        </is>
+      </c>
+      <c r="G96" t="inlineStr">
+        <is>
+          <t>2025-03-31</t>
+        </is>
+      </c>
+    </row>
+    <row r="97">
+      <c r="A97" t="inlineStr">
+        <is>
+          <t>M&amp;M'S Melk Chocolade Mini’s Snoepjes</t>
+        </is>
+      </c>
+      <c r="B97" t="inlineStr">
+        <is>
+          <t>3.39</t>
+        </is>
+      </c>
+      <c r="C97" t="inlineStr"/>
+      <c r="D97" t="inlineStr">
+        <is>
+          <t>Per 176 g</t>
+        </is>
+      </c>
+      <c r="E97" t="inlineStr">
+        <is>
+          <t>branded</t>
+        </is>
+      </c>
+      <c r="F97" t="inlineStr">
+        <is>
+          <t>Plus</t>
+        </is>
+      </c>
+      <c r="G97" t="inlineStr">
+        <is>
+          <t>2025-03-31</t>
+        </is>
+      </c>
+    </row>
+    <row r="98">
+      <c r="A98" t="inlineStr">
+        <is>
+          <t xml:space="preserve">M&amp;M'S Melk Chocolade Choco </t>
+        </is>
+      </c>
+      <c r="B98" t="inlineStr">
+        <is>
+          <t>2.29</t>
+        </is>
+      </c>
+      <c r="C98" t="inlineStr"/>
+      <c r="D98" t="inlineStr">
+        <is>
+          <t>Per 125 g</t>
+        </is>
+      </c>
+      <c r="E98" t="inlineStr">
+        <is>
+          <t>branded</t>
+        </is>
+      </c>
+      <c r="F98" t="inlineStr">
+        <is>
+          <t>Plus</t>
+        </is>
+      </c>
+      <c r="G98" t="inlineStr">
+        <is>
+          <t>2025-03-31</t>
+        </is>
+      </c>
+    </row>
+    <row r="99">
+      <c r="A99" t="inlineStr">
+        <is>
+          <t xml:space="preserve">M&amp;M'S Crispy Melk Chocolade </t>
+        </is>
+      </c>
+      <c r="B99" t="inlineStr">
+        <is>
+          <t>1.49</t>
+        </is>
+      </c>
+      <c r="C99" t="inlineStr"/>
+      <c r="D99" t="inlineStr">
+        <is>
+          <t>Per 77 g</t>
+        </is>
+      </c>
+      <c r="E99" t="inlineStr">
+        <is>
+          <t>branded</t>
+        </is>
+      </c>
+      <c r="F99" t="inlineStr">
+        <is>
+          <t>Plus</t>
+        </is>
+      </c>
+      <c r="G99" t="inlineStr">
+        <is>
+          <t>2025-03-31</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:G29"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>Title</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>Price</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>Promo Price</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>Weight</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>Category</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>Store</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>Timestamp</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>Bekijk AH Rozijn choco's</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>1.59</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>1.59</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>200 g</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>Non_Branded</t>
+        </is>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>AH</t>
+        </is>
+      </c>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t>2025-03-31</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>Bekijk AH Classic choco's</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>2.39</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>2.39</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>200 g</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>Non_Branded</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>AH</t>
+        </is>
+      </c>
+      <c r="G3" t="inlineStr">
+        <is>
+          <t>2025-03-31</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>Bekijk AH Hazelnoten choco's</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>2.19</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>2.19</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>200 g</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>Non_Branded</t>
+        </is>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>AH</t>
+        </is>
+      </c>
+      <c r="G4" t="inlineStr">
+        <is>
+          <t>2025-03-31</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>Bekijk AH Pindarotsjes melk</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>2.59</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>2.59</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>250 g</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>Non_Branded</t>
+        </is>
+      </c>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>AH</t>
+        </is>
+      </c>
+      <c r="G5" t="inlineStr">
+        <is>
+          <t>2025-03-31</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>Bekijk AH Crispy choco's</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>2.49</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>2.49</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>210 g</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>Non_Branded</t>
+        </is>
+      </c>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>AH</t>
+        </is>
+      </c>
+      <c r="G6" t="inlineStr">
+        <is>
+          <t>2025-03-31</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>Bekijk AH Pindarotsjes puur</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>2.59</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>2.59</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>250 g</t>
+        </is>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>Non_Branded</t>
+        </is>
+      </c>
+      <c r="F7" t="inlineStr">
+        <is>
+          <t>AH</t>
+        </is>
+      </c>
+      <c r="G7" t="inlineStr">
+        <is>
+          <t>2025-03-31</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>Bekijk AH Crunch choco's</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>2.39</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>2.39</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>175 g</t>
+        </is>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>Non_Branded</t>
+        </is>
+      </c>
+      <c r="F8" t="inlineStr">
+        <is>
+          <t>AH</t>
+        </is>
+      </c>
+      <c r="G8" t="inlineStr">
+        <is>
+          <t>2025-03-31</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>Bekijk AH Pindarotsjes melk</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>4.99</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>4.99</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>500 g</t>
+        </is>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>Non_Branded</t>
+        </is>
+      </c>
+      <c r="F9" t="inlineStr">
+        <is>
+          <t>AH</t>
+        </is>
+      </c>
+      <c r="G9" t="inlineStr">
+        <is>
+          <t>2025-03-31</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>Bekijk AH Pindarotsjes mix</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>4.99</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>4.99</t>
+        </is>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>500 g</t>
+        </is>
+      </c>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>Non_Branded</t>
+        </is>
+      </c>
+      <c r="F10" t="inlineStr">
+        <is>
+          <t>AH</t>
+        </is>
+      </c>
+      <c r="G10" t="inlineStr">
+        <is>
+          <t>2025-03-31</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>Bekijk AH Pindarotsjes wit</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>2.59</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>2.59</t>
+        </is>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>250 g</t>
+        </is>
+      </c>
+      <c r="E11" t="inlineStr">
+        <is>
+          <t>Non_Branded</t>
+        </is>
+      </c>
+      <c r="F11" t="inlineStr">
+        <is>
+          <t>AH</t>
+        </is>
+      </c>
+      <c r="G11" t="inlineStr">
+        <is>
+          <t>2025-03-31</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>Bekijk AH Pinda choco's</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>2.69</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>2.69</t>
+        </is>
+      </c>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>400 g</t>
+        </is>
+      </c>
+      <c r="E12" t="inlineStr">
+        <is>
+          <t>Non_Branded</t>
+        </is>
+      </c>
+      <c r="F12" t="inlineStr">
+        <is>
+          <t>AH</t>
+        </is>
+      </c>
+      <c r="G12" t="inlineStr">
+        <is>
+          <t>2025-03-31</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>Bekijk M&amp;M'S Melk chocolade party</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>12.49</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>12.49</t>
+        </is>
+      </c>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>1000 g</t>
+        </is>
+      </c>
+      <c r="E13" t="inlineStr">
+        <is>
+          <t>Branded</t>
+        </is>
+      </c>
+      <c r="F13" t="inlineStr">
+        <is>
+          <t>AH</t>
+        </is>
+      </c>
+      <c r="G13" t="inlineStr">
+        <is>
+          <t>2025-03-31</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>Bekijk M&amp;M'S Pinda melk chocolade party</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>12.49</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>12.49</t>
+        </is>
+      </c>
+      <c r="D14" t="inlineStr">
+        <is>
+          <t>1000 g</t>
+        </is>
+      </c>
+      <c r="E14" t="inlineStr">
+        <is>
+          <t>Branded</t>
+        </is>
+      </c>
+      <c r="F14" t="inlineStr">
+        <is>
+          <t>AH</t>
+        </is>
+      </c>
+      <c r="G14" t="inlineStr">
+        <is>
+          <t>2025-03-31</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>Bekijk M&amp;M'S Crispy melk chocolade party</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>12.49</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>12.49</t>
+        </is>
+      </c>
+      <c r="D15" t="inlineStr">
+        <is>
+          <t>850 g</t>
+        </is>
+      </c>
+      <c r="E15" t="inlineStr">
+        <is>
+          <t>Branded</t>
+        </is>
+      </c>
+      <c r="F15" t="inlineStr">
+        <is>
+          <t>AH</t>
+        </is>
+      </c>
+      <c r="G15" t="inlineStr">
+        <is>
+          <t>2025-03-31</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>Bekijk M&amp;M'S Chocolade snoepjes mix pakket</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>Oude prijs: €10.17</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>9.15</t>
+        </is>
+      </c>
+      <c r="D16" t="inlineStr">
+        <is>
+          <t>per pakket</t>
+        </is>
+      </c>
+      <c r="E16" t="inlineStr">
+        <is>
+          <t>Branded</t>
+        </is>
+      </c>
+      <c r="F16" t="inlineStr">
+        <is>
+          <t>AH</t>
+        </is>
+      </c>
+      <c r="G16" t="inlineStr">
+        <is>
+          <t>2025-03-31</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>Bekijk M&amp;M'S Gezouten karamel melk chocolade maxi</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>Oude prijs: €5.49</t>
+        </is>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>4.49</t>
+        </is>
+      </c>
+      <c r="D17" t="inlineStr">
+        <is>
+          <t>367 g</t>
+        </is>
+      </c>
+      <c r="E17" t="inlineStr">
+        <is>
+          <t>Branded</t>
+        </is>
+      </c>
+      <c r="F17" t="inlineStr">
+        <is>
+          <t>AH</t>
+        </is>
+      </c>
+      <c r="G17" t="inlineStr">
+        <is>
+          <t>2025-03-31</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>Bekijk M&amp;M'S Pinda melk chocolade maxi</t>
+        </is>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>Oude prijs: €5.39</t>
+        </is>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>4.49</t>
+        </is>
+      </c>
+      <c r="D18" t="inlineStr">
+        <is>
+          <t>400 g</t>
+        </is>
+      </c>
+      <c r="E18" t="inlineStr">
+        <is>
+          <t>Branded</t>
+        </is>
+      </c>
+      <c r="F18" t="inlineStr">
+        <is>
+          <t>AH</t>
+        </is>
+      </c>
+      <c r="G18" t="inlineStr">
+        <is>
+          <t>2025-03-31</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>Bekijk M&amp;M'S Crispy melkchocolade maxi</t>
+        </is>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>Oude prijs: €5.39</t>
+        </is>
+      </c>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>4.49</t>
+        </is>
+      </c>
+      <c r="D19" t="inlineStr">
+        <is>
+          <t>340 g</t>
+        </is>
+      </c>
+      <c r="E19" t="inlineStr">
+        <is>
+          <t>Branded</t>
+        </is>
+      </c>
+      <c r="F19" t="inlineStr">
+        <is>
+          <t>AH</t>
+        </is>
+      </c>
+      <c r="G19" t="inlineStr">
+        <is>
+          <t>2025-03-31</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>Bekijk M&amp;M'S Melk chocolade</t>
+        </is>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>Oude prijs: €5.39</t>
+        </is>
+      </c>
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>4.49</t>
+        </is>
+      </c>
+      <c r="D20" t="inlineStr">
+        <is>
+          <t>400 g</t>
+        </is>
+      </c>
+      <c r="E20" t="inlineStr">
+        <is>
+          <t>Branded</t>
+        </is>
+      </c>
+      <c r="F20" t="inlineStr">
+        <is>
+          <t>AH</t>
+        </is>
+      </c>
+      <c r="G20" t="inlineStr">
+        <is>
+          <t>2025-03-31</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>Bekijk M&amp;M'S Minis melk chocolade</t>
+        </is>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>3.39</t>
+        </is>
+      </c>
+      <c r="C21" t="inlineStr">
+        <is>
+          <t>3.39</t>
+        </is>
+      </c>
+      <c r="D21" t="inlineStr">
+        <is>
+          <t>176 g</t>
+        </is>
+      </c>
+      <c r="E21" t="inlineStr">
+        <is>
+          <t>Branded</t>
+        </is>
+      </c>
+      <c r="F21" t="inlineStr">
+        <is>
+          <t>AH</t>
+        </is>
+      </c>
+      <c r="G21" t="inlineStr">
+        <is>
+          <t>2025-03-31</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>Bekijk M&amp;M'S Crispy melk chocolade</t>
+        </is>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>3.39</t>
+        </is>
+      </c>
+      <c r="C22" t="inlineStr">
+        <is>
+          <t>3.39</t>
+        </is>
+      </c>
+      <c r="D22" t="inlineStr">
+        <is>
+          <t>187 g</t>
+        </is>
+      </c>
+      <c r="E22" t="inlineStr">
+        <is>
+          <t>Branded</t>
+        </is>
+      </c>
+      <c r="F22" t="inlineStr">
+        <is>
+          <t>AH</t>
+        </is>
+      </c>
+      <c r="G22" t="inlineStr">
+        <is>
+          <t>2025-03-31</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>Bekijk M&amp;M'S Pinda melk chocolade</t>
+        </is>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>3.39</t>
+        </is>
+      </c>
+      <c r="C23" t="inlineStr">
+        <is>
+          <t>3.39</t>
+        </is>
+      </c>
+      <c r="D23" t="inlineStr">
+        <is>
+          <t>200 g</t>
+        </is>
+      </c>
+      <c r="E23" t="inlineStr">
+        <is>
+          <t>Branded</t>
+        </is>
+      </c>
+      <c r="F23" t="inlineStr">
+        <is>
+          <t>AH</t>
+        </is>
+      </c>
+      <c r="G23" t="inlineStr">
+        <is>
+          <t>2025-03-31</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>Bekijk M&amp;M'S Melk chocolade</t>
+        </is>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>3.39</t>
+        </is>
+      </c>
+      <c r="C24" t="inlineStr">
+        <is>
+          <t>3.39</t>
+        </is>
+      </c>
+      <c r="D24" t="inlineStr">
+        <is>
+          <t>200 g</t>
+        </is>
+      </c>
+      <c r="E24" t="inlineStr">
+        <is>
+          <t>Branded</t>
+        </is>
+      </c>
+      <c r="F24" t="inlineStr">
+        <is>
+          <t>AH</t>
+        </is>
+      </c>
+      <c r="G24" t="inlineStr">
+        <is>
+          <t>2025-03-31</t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="inlineStr">
+        <is>
+          <t>Bekijk M&amp;M'S Gezouten karamel melk chocolade</t>
+        </is>
+      </c>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>2.95</t>
+        </is>
+      </c>
+      <c r="C25" t="inlineStr">
+        <is>
+          <t>2.95</t>
+        </is>
+      </c>
+      <c r="D25" t="inlineStr">
+        <is>
+          <t>176 g</t>
+        </is>
+      </c>
+      <c r="E25" t="inlineStr">
+        <is>
+          <t>Branded</t>
+        </is>
+      </c>
+      <c r="F25" t="inlineStr">
+        <is>
+          <t>AH</t>
+        </is>
+      </c>
+      <c r="G25" t="inlineStr">
+        <is>
+          <t>2025-03-31</t>
+        </is>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="inlineStr">
+        <is>
+          <t>Bekijk M&amp;M'S Pinda melk chocolade</t>
+        </is>
+      </c>
+      <c r="B26" t="inlineStr">
+        <is>
+          <t>2.29</t>
+        </is>
+      </c>
+      <c r="C26" t="inlineStr">
+        <is>
+          <t>2.29</t>
+        </is>
+      </c>
+      <c r="D26" t="inlineStr">
+        <is>
+          <t>125 g</t>
+        </is>
+      </c>
+      <c r="E26" t="inlineStr">
+        <is>
+          <t>Branded</t>
+        </is>
+      </c>
+      <c r="F26" t="inlineStr">
+        <is>
+          <t>AH</t>
+        </is>
+      </c>
+      <c r="G26" t="inlineStr">
+        <is>
+          <t>2025-03-31</t>
+        </is>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="inlineStr">
+        <is>
+          <t>Bekijk M&amp;M'S Melk chocolade</t>
+        </is>
+      </c>
+      <c r="B27" t="inlineStr">
+        <is>
+          <t>2.29</t>
+        </is>
+      </c>
+      <c r="C27" t="inlineStr">
+        <is>
+          <t>2.29</t>
+        </is>
+      </c>
+      <c r="D27" t="inlineStr">
+        <is>
+          <t>125 g</t>
+        </is>
+      </c>
+      <c r="E27" t="inlineStr">
+        <is>
+          <t>Branded</t>
+        </is>
+      </c>
+      <c r="F27" t="inlineStr">
+        <is>
+          <t>AH</t>
+        </is>
+      </c>
+      <c r="G27" t="inlineStr">
+        <is>
+          <t>2025-03-31</t>
+        </is>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="inlineStr">
+        <is>
+          <t>Bekijk M&amp;M'S Crispy melk chocolade</t>
+        </is>
+      </c>
+      <c r="B28" t="inlineStr">
+        <is>
+          <t>2.29</t>
+        </is>
+      </c>
+      <c r="C28" t="inlineStr">
+        <is>
+          <t>2.29</t>
+        </is>
+      </c>
+      <c r="D28" t="inlineStr">
+        <is>
+          <t>107 g</t>
+        </is>
+      </c>
+      <c r="E28" t="inlineStr">
+        <is>
+          <t>Branded</t>
+        </is>
+      </c>
+      <c r="F28" t="inlineStr">
+        <is>
+          <t>AH</t>
+        </is>
+      </c>
+      <c r="G28" t="inlineStr">
+        <is>
+          <t>2025-03-31</t>
+        </is>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="inlineStr">
+        <is>
+          <t>Bekijk M&amp;M'S Pinda melk chocolade</t>
+        </is>
+      </c>
+      <c r="B29" t="inlineStr">
+        <is>
+          <t>1.49</t>
+        </is>
+      </c>
+      <c r="C29" t="inlineStr">
+        <is>
+          <t>1.49</t>
+        </is>
+      </c>
+      <c r="D29" t="inlineStr">
+        <is>
+          <t>45 g</t>
+        </is>
+      </c>
+      <c r="E29" t="inlineStr">
+        <is>
+          <t>Branded</t>
+        </is>
+      </c>
+      <c r="F29" t="inlineStr">
+        <is>
+          <t>AH</t>
+        </is>
+      </c>
+      <c r="G29" t="inlineStr">
+        <is>
+          <t>2025-03-31</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
added new items for aldi
</commit_message>
<xml_diff>
--- a/Web Scraping/choco.xlsx
+++ b/Web Scraping/choco.xlsx
@@ -414,7 +414,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G75"/>
+  <dimension ref="A1:G88"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -462,7 +462,7 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Jumbo Choco Crispies 210 g</t>
+          <t>Jumbo Choco Classic 200 g</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
@@ -472,12 +472,12 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>2,43</t>
+          <t>2,34</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>210 g</t>
+          <t>200 g</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
@@ -492,14 +492,14 @@
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>2025-07-07</t>
+          <t>2025-07-21</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Jumbo Choco Classic 200 g</t>
+          <t>Jumbo Choco Pinda's 250g</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
@@ -509,12 +509,12 @@
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>2,34</t>
+          <t>2,09</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>200 g</t>
+          <t>250 g</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
@@ -529,14 +529,14 @@
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>2025-07-07</t>
+          <t>2025-07-21</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Jumbo Melkchocolade Pindarotsjes 250 g</t>
+          <t>Jumbo Choco Crispies 210 g</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
@@ -551,7 +551,7 @@
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>250 g</t>
+          <t>210 g</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
@@ -566,14 +566,14 @@
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>2025-07-07</t>
+          <t>2025-07-21</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Jumbo Choco Pinda's 250g</t>
+          <t>Jumbo Melkchocolade Pindarotsjes 250 g</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
@@ -583,12 +583,12 @@
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>2,09</t>
+          <t>2,43</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>Weight not found</t>
+          <t>250 g</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
@@ -603,14 +603,14 @@
       </c>
       <c r="G5" t="inlineStr">
         <is>
-          <t>2025-07-07</t>
+          <t>2025-07-21</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>Jumbo Choco Ballen Hazelnoot Melk 200 g</t>
+          <t>Jumbo Choco Crunch 175 g</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
@@ -620,12 +620,12 @@
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>2,17</t>
+          <t>2,34</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>200 g</t>
+          <t>175 g</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
@@ -640,14 +640,14 @@
       </c>
       <c r="G6" t="inlineStr">
         <is>
-          <t>2025-07-07</t>
+          <t>2025-07-21</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>Jumbo Choco Crunch 175 g</t>
+          <t>Jumbo Choco Pinda's 400 g</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
@@ -657,12 +657,12 @@
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>2,34</t>
+          <t>2,66</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>175 g</t>
+          <t>400 g</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
@@ -677,14 +677,14 @@
       </c>
       <c r="G7" t="inlineStr">
         <is>
-          <t>2025-07-07</t>
+          <t>2025-07-21</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>Jumbo Musket Flikken 150 g</t>
+          <t>Jumbo Pindarotsjes Puur 250 g</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
@@ -694,12 +694,12 @@
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>2,24</t>
+          <t>2,43</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>150 g</t>
+          <t>250 g</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
@@ -714,14 +714,14 @@
       </c>
       <c r="G8" t="inlineStr">
         <is>
-          <t>2025-07-07</t>
+          <t>2025-07-21</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>Jumbo Chocolade Oublies 150 g</t>
+          <t>Jumbo Choco Ballen Hazelnoot Melk 200 g</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
@@ -731,12 +731,12 @@
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>2,29</t>
+          <t>2,17</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>150 g</t>
+          <t>200 g</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
@@ -751,14 +751,14 @@
       </c>
       <c r="G9" t="inlineStr">
         <is>
-          <t>2025-07-07</t>
+          <t>2025-07-21</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>Jumbo Choco Pinda's 400 g</t>
+          <t>Jumbo Musket Flikken 150 g</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
@@ -768,12 +768,12 @@
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>2,66</t>
+          <t>2,24</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>400 g</t>
+          <t>150 g</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
@@ -788,14 +788,14 @@
       </c>
       <c r="G10" t="inlineStr">
         <is>
-          <t>2025-07-07</t>
+          <t>2025-07-21</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>Jumbo Choco Rozijnen Melk 200 g</t>
+          <t>Jumbo Chocolade Oublies 150 g</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
@@ -805,12 +805,12 @@
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>1,67</t>
+          <t>2,29</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>200 g</t>
+          <t>150 g</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
@@ -825,14 +825,14 @@
       </c>
       <c r="G11" t="inlineStr">
         <is>
-          <t>2025-07-07</t>
+          <t>2025-07-21</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>Jumbo Pindarotsjes Puur 250 g</t>
+          <t>Jumbo Mokka Boontjes Puur 125 g</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
@@ -842,12 +842,12 @@
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>2,43</t>
+          <t>2,15</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>250 g</t>
+          <t>125 g</t>
         </is>
       </c>
       <c r="E12" t="inlineStr">
@@ -862,7 +862,7 @@
       </c>
       <c r="G12" t="inlineStr">
         <is>
-          <t>2025-07-07</t>
+          <t>2025-07-21</t>
         </is>
       </c>
     </row>
@@ -879,7 +879,7 @@
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>1,49</t>
+          <t>1,79</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
@@ -899,7 +899,7 @@
       </c>
       <c r="G13" t="inlineStr">
         <is>
-          <t>2025-07-07</t>
+          <t>2025-07-21</t>
         </is>
       </c>
     </row>
@@ -931,7 +931,7 @@
       </c>
       <c r="G14" t="inlineStr">
         <is>
-          <t>2025-07-07</t>
+          <t>2025-07-21</t>
         </is>
       </c>
     </row>
@@ -963,7 +963,7 @@
       </c>
       <c r="G15" t="inlineStr">
         <is>
-          <t>2025-07-07</t>
+          <t>2025-07-21</t>
         </is>
       </c>
     </row>
@@ -995,7 +995,7 @@
       </c>
       <c r="G16" t="inlineStr">
         <is>
-          <t>2025-07-07</t>
+          <t>2025-07-21</t>
         </is>
       </c>
     </row>
@@ -1027,7 +1027,7 @@
       </c>
       <c r="G17" t="inlineStr">
         <is>
-          <t>2025-07-07</t>
+          <t>2025-07-21</t>
         </is>
       </c>
     </row>
@@ -1059,7 +1059,7 @@
       </c>
       <c r="G18" t="inlineStr">
         <is>
-          <t>2025-07-07</t>
+          <t>2025-07-21</t>
         </is>
       </c>
     </row>
@@ -1091,7 +1091,7 @@
       </c>
       <c r="G19" t="inlineStr">
         <is>
-          <t>2025-07-07</t>
+          <t>2025-07-21</t>
         </is>
       </c>
     </row>
@@ -1123,7 +1123,7 @@
       </c>
       <c r="G20" t="inlineStr">
         <is>
-          <t>2025-07-07</t>
+          <t>2025-07-21</t>
         </is>
       </c>
     </row>
@@ -1155,7 +1155,7 @@
       </c>
       <c r="G21" t="inlineStr">
         <is>
-          <t>2025-07-07</t>
+          <t>2025-07-21</t>
         </is>
       </c>
     </row>
@@ -1192,19 +1192,19 @@
       </c>
       <c r="G22" t="inlineStr">
         <is>
-          <t>2025-07-07</t>
+          <t>2025-07-21</t>
         </is>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>1 de Beste Choconino</t>
+          <t>1 de Beste Nino's</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>1,79</t>
+          <t>1,89</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
@@ -1229,7 +1229,7 @@
       </c>
       <c r="G23" t="inlineStr">
         <is>
-          <t>2025-07-07</t>
+          <t>2025-07-21</t>
         </is>
       </c>
     </row>
@@ -1266,7 +1266,7 @@
       </c>
       <c r="G24" t="inlineStr">
         <is>
-          <t>2025-07-07</t>
+          <t>2025-07-21</t>
         </is>
       </c>
     </row>
@@ -1303,7 +1303,7 @@
       </c>
       <c r="G25" t="inlineStr">
         <is>
-          <t>2025-07-07</t>
+          <t>2025-07-21</t>
         </is>
       </c>
     </row>
@@ -1340,7 +1340,7 @@
       </c>
       <c r="G26" t="inlineStr">
         <is>
-          <t>2025-07-07</t>
+          <t>2025-07-21</t>
         </is>
       </c>
     </row>
@@ -1377,7 +1377,7 @@
       </c>
       <c r="G27" t="inlineStr">
         <is>
-          <t>2025-07-07</t>
+          <t>2025-07-21</t>
         </is>
       </c>
     </row>
@@ -1414,7 +1414,7 @@
       </c>
       <c r="G28" t="inlineStr">
         <is>
-          <t>2025-07-07</t>
+          <t>2025-07-21</t>
         </is>
       </c>
     </row>
@@ -1451,7 +1451,7 @@
       </c>
       <c r="G29" t="inlineStr">
         <is>
-          <t>2025-07-07</t>
+          <t>2025-07-21</t>
         </is>
       </c>
     </row>
@@ -1463,7 +1463,7 @@
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>1,48</t>
+          <t>1,75</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
@@ -1488,7 +1488,7 @@
       </c>
       <c r="G30" t="inlineStr">
         <is>
-          <t>2025-07-07</t>
+          <t>2025-07-21</t>
         </is>
       </c>
     </row>
@@ -1525,19 +1525,19 @@
       </c>
       <c r="G31" t="inlineStr">
         <is>
-          <t>2025-07-07</t>
+          <t>2025-07-21</t>
         </is>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>Ovaal drie chocolades 900 ml</t>
+          <t>G'woon choco classic</t>
         </is>
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>2.99</t>
+          <t>1.75</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
@@ -1562,19 +1562,19 @@
       </c>
       <c r="G32" t="inlineStr">
         <is>
-          <t>2025-07-07</t>
+          <t>2025-07-21</t>
         </is>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>G'woon choco classic</t>
+          <t>G'woon choco ruitjes</t>
         </is>
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>1.75</t>
+          <t>1.99</t>
         </is>
       </c>
       <c r="C33" t="inlineStr">
@@ -1599,19 +1599,19 @@
       </c>
       <c r="G33" t="inlineStr">
         <is>
-          <t>2025-07-07</t>
+          <t>2025-07-21</t>
         </is>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>G'woon dip cookie choco 200gr</t>
+          <t>G'woon choco pinda 250gr</t>
         </is>
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>2.39</t>
+          <t>1.55</t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
@@ -1636,19 +1636,19 @@
       </c>
       <c r="G34" t="inlineStr">
         <is>
-          <t>2025-07-07</t>
+          <t>2025-07-21</t>
         </is>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>G'woon choco ruitjes</t>
+          <t>G'woon chocoprentjes melk</t>
         </is>
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>1.99</t>
+          <t>1.59</t>
         </is>
       </c>
       <c r="C35" t="inlineStr">
@@ -1673,19 +1673,19 @@
       </c>
       <c r="G35" t="inlineStr">
         <is>
-          <t>2025-07-07</t>
+          <t>2025-07-21</t>
         </is>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>G'woon choco pinda 250gr</t>
+          <t>G'woon choco crunch 150gr</t>
         </is>
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>1.55</t>
+          <t>1.57</t>
         </is>
       </c>
       <c r="C36" t="inlineStr">
@@ -1710,19 +1710,19 @@
       </c>
       <c r="G36" t="inlineStr">
         <is>
-          <t>2025-07-07</t>
+          <t>2025-07-21</t>
         </is>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>G'woon chocoprentjes melk</t>
+          <t>G'woon mini choco amandel 8st</t>
         </is>
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>1.59</t>
+          <t>2.49</t>
         </is>
       </c>
       <c r="C37" t="inlineStr">
@@ -1747,19 +1747,19 @@
       </c>
       <c r="G37" t="inlineStr">
         <is>
-          <t>2025-07-07</t>
+          <t>2025-07-21</t>
         </is>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>G'woon choco crunch 150gr</t>
+          <t>G'woon biscuit duo choco 500gr</t>
         </is>
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>1.57</t>
+          <t>1.39</t>
         </is>
       </c>
       <c r="C38" t="inlineStr">
@@ -1784,19 +1784,19 @@
       </c>
       <c r="G38" t="inlineStr">
         <is>
-          <t>2025-07-07</t>
+          <t>2025-07-21</t>
         </is>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>G'woon mini choco amandel 8st</t>
+          <t>G'woon pindakoek melkchocolade</t>
         </is>
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>2.49</t>
+          <t>1.87</t>
         </is>
       </c>
       <c r="C39" t="inlineStr">
@@ -1821,19 +1821,19 @@
       </c>
       <c r="G39" t="inlineStr">
         <is>
-          <t>2025-07-07</t>
+          <t>2025-07-21</t>
         </is>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>G'woon biscuit duo choco 500gr</t>
+          <t>G'woon choco hazelnoot 200gr</t>
         </is>
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>1.39</t>
+          <t>1.94</t>
         </is>
       </c>
       <c r="C40" t="inlineStr">
@@ -1858,19 +1858,19 @@
       </c>
       <c r="G40" t="inlineStr">
         <is>
-          <t>2025-07-07</t>
+          <t>2025-07-21</t>
         </is>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>G'woon pindakoek melkchocolade</t>
+          <t>G'woon choco rozijnen 200 gr</t>
         </is>
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>1.87</t>
+          <t>1.49</t>
         </is>
       </c>
       <c r="C41" t="inlineStr">
@@ -1895,19 +1895,19 @@
       </c>
       <c r="G41" t="inlineStr">
         <is>
-          <t>2025-07-07</t>
+          <t>2025-07-21</t>
         </is>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>G'woon choco hazelnoot 200gr</t>
+          <t>G'woon choco crisp 210 gr</t>
         </is>
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>1.94</t>
+          <t>2.19</t>
         </is>
       </c>
       <c r="C42" t="inlineStr">
@@ -1932,19 +1932,19 @@
       </c>
       <c r="G42" t="inlineStr">
         <is>
-          <t>2025-07-07</t>
+          <t>2025-07-21</t>
         </is>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>G'woon choco rozijnen 200 gr</t>
+          <t>G'woon granenbiscuit choco 292gr</t>
         </is>
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>1.49</t>
+          <t>1.79</t>
         </is>
       </c>
       <c r="C43" t="inlineStr">
@@ -1969,19 +1969,19 @@
       </c>
       <c r="G43" t="inlineStr">
         <is>
-          <t>2025-07-07</t>
+          <t>2025-07-21</t>
         </is>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>G'woon choco crisp 210 gr</t>
+          <t>G'woon choco schelpjes 500gr</t>
         </is>
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>2.19</t>
+          <t>1.59</t>
         </is>
       </c>
       <c r="C44" t="inlineStr">
@@ -2006,7 +2006,7 @@
       </c>
       <c r="G44" t="inlineStr">
         <is>
-          <t>2025-07-07</t>
+          <t>2025-07-21</t>
         </is>
       </c>
     </row>
@@ -2043,19 +2043,19 @@
       </c>
       <c r="G45" t="inlineStr">
         <is>
-          <t>2025-07-07</t>
+          <t>2025-07-21</t>
         </is>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>G'woon granenbiscuit choco 292gr</t>
+          <t>G'woon chocosticks vanille 12</t>
         </is>
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>1.79</t>
+          <t>1.89</t>
         </is>
       </c>
       <c r="C46" t="inlineStr">
@@ -2080,19 +2080,19 @@
       </c>
       <c r="G46" t="inlineStr">
         <is>
-          <t>2025-07-07</t>
+          <t>2025-07-21</t>
         </is>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>G'woon chocosticks vanille 12</t>
+          <t>G'woon chocoprentjes puur</t>
         </is>
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>1.95</t>
+          <t>1.49</t>
         </is>
       </c>
       <c r="C47" t="inlineStr">
@@ -2117,19 +2117,19 @@
       </c>
       <c r="G47" t="inlineStr">
         <is>
-          <t>2025-07-07</t>
+          <t>2025-07-21</t>
         </is>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>G'woon chocoprentjes puur</t>
+          <t>G'woon choco chocos 500gr</t>
         </is>
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>1.49</t>
+          <t>1.59</t>
         </is>
       </c>
       <c r="C48" t="inlineStr">
@@ -2154,19 +2154,19 @@
       </c>
       <c r="G48" t="inlineStr">
         <is>
-          <t>2025-07-07</t>
+          <t>2025-07-21</t>
         </is>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>G'woon choconino 5 stuks</t>
+          <t>G'woon krokante muesli choco 900gr</t>
         </is>
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>1.89</t>
+          <t>2.99</t>
         </is>
       </c>
       <c r="C49" t="inlineStr">
@@ -2191,19 +2191,19 @@
       </c>
       <c r="G49" t="inlineStr">
         <is>
-          <t>2025-07-07</t>
+          <t>2025-07-21</t>
         </is>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t>G'woon mega choco's amandel 6s</t>
+          <t>G'woon choconino 5 stuks</t>
         </is>
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>3.45</t>
+          <t>1.89</t>
         </is>
       </c>
       <c r="C50" t="inlineStr">
@@ -2228,19 +2228,19 @@
       </c>
       <c r="G50" t="inlineStr">
         <is>
-          <t>2025-07-07</t>
+          <t>2025-07-21</t>
         </is>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="inlineStr">
         <is>
-          <t>G'woon mega choco's wit 6st</t>
+          <t>G'woon mega choco's amandel 6s</t>
         </is>
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>3.49</t>
+          <t>3.45</t>
         </is>
       </c>
       <c r="C51" t="inlineStr">
@@ -2265,19 +2265,19 @@
       </c>
       <c r="G51" t="inlineStr">
         <is>
-          <t>2025-07-07</t>
+          <t>2025-07-21</t>
         </is>
       </c>
     </row>
     <row r="52">
       <c r="A52" t="inlineStr">
         <is>
-          <t>G'woon mega choco's melk 6st</t>
+          <t>G'woon mega choco's wit 6st</t>
         </is>
       </c>
       <c r="B52" t="inlineStr">
         <is>
-          <t>3.39</t>
+          <t>3.49</t>
         </is>
       </c>
       <c r="C52" t="inlineStr">
@@ -2302,29 +2302,29 @@
       </c>
       <c r="G52" t="inlineStr">
         <is>
-          <t>2025-07-07</t>
+          <t>2025-07-21</t>
         </is>
       </c>
     </row>
     <row r="53">
       <c r="A53" t="inlineStr">
         <is>
-          <t>Pindarotsjes</t>
+          <t>G'woon mega choco's melk 6st</t>
         </is>
       </c>
       <c r="B53" t="inlineStr">
         <is>
-          <t>2.39</t>
+          <t>3.39</t>
         </is>
       </c>
       <c r="C53" t="inlineStr">
         <is>
-          <t>No promo price</t>
+          <t>Promo price not found</t>
         </is>
       </c>
       <c r="D53" t="inlineStr">
         <is>
-          <t>250 g</t>
+          <t>Weight not found</t>
         </is>
       </c>
       <c r="E53" t="inlineStr">
@@ -2334,24 +2334,24 @@
       </c>
       <c r="F53" t="inlineStr">
         <is>
-          <t>Aldi</t>
+          <t>Vomar</t>
         </is>
       </c>
       <c r="G53" t="inlineStr">
         <is>
-          <t>2025-07-07</t>
+          <t>2025-07-21</t>
         </is>
       </c>
     </row>
     <row r="54">
       <c r="A54" t="inlineStr">
         <is>
-          <t>Mini-mix power</t>
+          <t>Pindarotsjes</t>
         </is>
       </c>
       <c r="B54" t="inlineStr">
         <is>
-          <t>3.49</t>
+          <t>2.39</t>
         </is>
       </c>
       <c r="C54" t="inlineStr">
@@ -2361,7 +2361,7 @@
       </c>
       <c r="D54" t="inlineStr">
         <is>
-          <t>Inhoud: ca. 28 stuks, 500 g</t>
+          <t>250 g</t>
         </is>
       </c>
       <c r="E54" t="inlineStr">
@@ -2376,7 +2376,7 @@
       </c>
       <c r="G54" t="inlineStr">
         <is>
-          <t>2025-07-07</t>
+          <t>2025-07-21</t>
         </is>
       </c>
     </row>
@@ -2413,7 +2413,7 @@
       </c>
       <c r="G55" t="inlineStr">
         <is>
-          <t>2025-07-07</t>
+          <t>2025-07-21</t>
         </is>
       </c>
     </row>
@@ -2450,7 +2450,7 @@
       </c>
       <c r="G56" t="inlineStr">
         <is>
-          <t>2025-07-07</t>
+          <t>2025-07-21</t>
         </is>
       </c>
     </row>
@@ -2487,19 +2487,19 @@
       </c>
       <c r="G57" t="inlineStr">
         <is>
-          <t>2025-07-07</t>
+          <t>2025-07-21</t>
         </is>
       </c>
     </row>
     <row r="58">
       <c r="A58" t="inlineStr">
         <is>
-          <t>Pindarotsjes</t>
+          <t>Roomboter amandelharten of pindakoeken</t>
         </is>
       </c>
       <c r="B58" t="inlineStr">
         <is>
-          <t>2.39</t>
+          <t>2.99</t>
         </is>
       </c>
       <c r="C58" t="inlineStr">
@@ -2509,7 +2509,7 @@
       </c>
       <c r="D58" t="inlineStr">
         <is>
-          <t>250 g</t>
+          <t>300 g</t>
         </is>
       </c>
       <c r="E58" t="inlineStr">
@@ -2524,44 +2524,44 @@
       </c>
       <c r="G58" t="inlineStr">
         <is>
-          <t>2025-07-07</t>
+          <t>2025-07-21</t>
         </is>
       </c>
     </row>
     <row r="59">
       <c r="A59" t="inlineStr">
         <is>
-          <t>M&amp;M'S Pinda chocolade snoepjes maxi 400g</t>
+          <t>Pindarotsjes</t>
         </is>
       </c>
       <c r="B59" t="inlineStr">
         <is>
-          <t>Promo price not found</t>
+          <t>2.39</t>
         </is>
       </c>
       <c r="C59" t="inlineStr">
         <is>
-          <t>5,69</t>
+          <t>No promo price</t>
         </is>
       </c>
       <c r="D59" t="inlineStr">
         <is>
-          <t>400 g</t>
+          <t>250 g</t>
         </is>
       </c>
       <c r="E59" t="inlineStr">
         <is>
-          <t>branded</t>
+          <t>Non_Branded</t>
         </is>
       </c>
       <c r="F59" t="inlineStr">
         <is>
-          <t>Jumbo</t>
+          <t>Aldi</t>
         </is>
       </c>
       <c r="G59" t="inlineStr">
         <is>
-          <t>2025-07-07</t>
+          <t>2025-07-21</t>
         </is>
       </c>
     </row>
@@ -2578,7 +2578,7 @@
       </c>
       <c r="C60" t="inlineStr">
         <is>
-          <t>9,99</t>
+          <t>9,39</t>
         </is>
       </c>
       <c r="D60" t="inlineStr">
@@ -2598,14 +2598,14 @@
       </c>
       <c r="G60" t="inlineStr">
         <is>
-          <t>2025-07-07</t>
+          <t>2025-07-21</t>
         </is>
       </c>
     </row>
     <row r="61">
       <c r="A61" t="inlineStr">
         <is>
-          <t>M&amp;M'S Crispy chocolade snoepjes partyzak 675g</t>
+          <t>M&amp;M'S Pinda chocolade snoepjes maxi 400g</t>
         </is>
       </c>
       <c r="B61" t="inlineStr">
@@ -2615,12 +2615,12 @@
       </c>
       <c r="C61" t="inlineStr">
         <is>
-          <t>9,99</t>
+          <t>5,69</t>
         </is>
       </c>
       <c r="D61" t="inlineStr">
         <is>
-          <t>675 g</t>
+          <t>400 g</t>
         </is>
       </c>
       <c r="E61" t="inlineStr">
@@ -2635,14 +2635,14 @@
       </c>
       <c r="G61" t="inlineStr">
         <is>
-          <t>2025-07-07</t>
+          <t>2025-07-21</t>
         </is>
       </c>
     </row>
     <row r="62">
       <c r="A62" t="inlineStr">
         <is>
-          <t>M&amp;M'S Melk Chocolade Pinda Snoepjes Zak Middel</t>
+          <t>M&amp;M'S Choco chocolade snoepjes partyzak 800g</t>
         </is>
       </c>
       <c r="B62" t="inlineStr">
@@ -2652,12 +2652,12 @@
       </c>
       <c r="C62" t="inlineStr">
         <is>
-          <t>3,09</t>
+          <t>9,39</t>
         </is>
       </c>
       <c r="D62" t="inlineStr">
         <is>
-          <t>200 g</t>
+          <t>800 g</t>
         </is>
       </c>
       <c r="E62" t="inlineStr">
@@ -2672,14 +2672,14 @@
       </c>
       <c r="G62" t="inlineStr">
         <is>
-          <t>2025-07-07</t>
+          <t>2025-07-21</t>
         </is>
       </c>
     </row>
     <row r="63">
       <c r="A63" t="inlineStr">
         <is>
-          <t>M&amp;M'S Crispy chocolade snoepjes maxi 340g</t>
+          <t>M&amp;M'S Crispy chocolade snoepjes partyzak 675g</t>
         </is>
       </c>
       <c r="B63" t="inlineStr">
@@ -2689,12 +2689,12 @@
       </c>
       <c r="C63" t="inlineStr">
         <is>
-          <t>5,18</t>
+          <t>9,89</t>
         </is>
       </c>
       <c r="D63" t="inlineStr">
         <is>
-          <t>340 g</t>
+          <t>675 g</t>
         </is>
       </c>
       <c r="E63" t="inlineStr">
@@ -2709,7 +2709,7 @@
       </c>
       <c r="G63" t="inlineStr">
         <is>
-          <t>2025-07-07</t>
+          <t>2025-07-21</t>
         </is>
       </c>
     </row>
@@ -2746,14 +2746,14 @@
       </c>
       <c r="G64" t="inlineStr">
         <is>
-          <t>2025-07-07</t>
+          <t>2025-07-21</t>
         </is>
       </c>
     </row>
     <row r="65">
       <c r="A65" t="inlineStr">
         <is>
-          <t>M&amp;M'S Choco chocolade snoepjes partyzak 800g</t>
+          <t>M&amp;M'S Melk Chocolade Pinda Snoepjes Zak Middel</t>
         </is>
       </c>
       <c r="B65" t="inlineStr">
@@ -2763,12 +2763,12 @@
       </c>
       <c r="C65" t="inlineStr">
         <is>
-          <t>9,99</t>
+          <t>3,09</t>
         </is>
       </c>
       <c r="D65" t="inlineStr">
         <is>
-          <t>800 g</t>
+          <t>200 g</t>
         </is>
       </c>
       <c r="E65" t="inlineStr">
@@ -2783,14 +2783,14 @@
       </c>
       <c r="G65" t="inlineStr">
         <is>
-          <t>2025-07-07</t>
+          <t>2025-07-21</t>
         </is>
       </c>
     </row>
     <row r="66">
       <c r="A66" t="inlineStr">
         <is>
-          <t>M&amp;M'S Crispy chocolade snoepjes 187g</t>
+          <t>M&amp;M'S Crispy chocolade snoepjes maxi 340g</t>
         </is>
       </c>
       <c r="B66" t="inlineStr">
@@ -2800,12 +2800,12 @@
       </c>
       <c r="C66" t="inlineStr">
         <is>
-          <t>3,09</t>
+          <t>5,18</t>
         </is>
       </c>
       <c r="D66" t="inlineStr">
         <is>
-          <t>187 g</t>
+          <t>340 g</t>
         </is>
       </c>
       <c r="E66" t="inlineStr">
@@ -2820,14 +2820,14 @@
       </c>
       <c r="G66" t="inlineStr">
         <is>
-          <t>2025-07-07</t>
+          <t>2025-07-21</t>
         </is>
       </c>
     </row>
     <row r="67">
       <c r="A67" t="inlineStr">
         <is>
-          <t>M&amp;M'S Choco chocolade snoepjes 125g</t>
+          <t>M&amp;M'S Crispy chocolade snoepjes 187g</t>
         </is>
       </c>
       <c r="B67" t="inlineStr">
@@ -2837,12 +2837,12 @@
       </c>
       <c r="C67" t="inlineStr">
         <is>
-          <t>2,09</t>
+          <t>3,09</t>
         </is>
       </c>
       <c r="D67" t="inlineStr">
         <is>
-          <t>125 g</t>
+          <t>187 g</t>
         </is>
       </c>
       <c r="E67" t="inlineStr">
@@ -2857,14 +2857,14 @@
       </c>
       <c r="G67" t="inlineStr">
         <is>
-          <t>2025-07-07</t>
+          <t>2025-07-21</t>
         </is>
       </c>
     </row>
     <row r="68">
       <c r="A68" t="inlineStr">
         <is>
-          <t>M&amp;M'S Choco chocolade snoepjes 200g</t>
+          <t>M&amp;M'S Pinda chocolade snoepjes 125g</t>
         </is>
       </c>
       <c r="B68" t="inlineStr">
@@ -2874,12 +2874,12 @@
       </c>
       <c r="C68" t="inlineStr">
         <is>
-          <t>3,09</t>
+          <t>2,08</t>
         </is>
       </c>
       <c r="D68" t="inlineStr">
         <is>
-          <t>200 g</t>
+          <t>125 g</t>
         </is>
       </c>
       <c r="E68" t="inlineStr">
@@ -2894,14 +2894,14 @@
       </c>
       <c r="G68" t="inlineStr">
         <is>
-          <t>2025-07-07</t>
+          <t>2025-07-21</t>
         </is>
       </c>
     </row>
     <row r="69">
       <c r="A69" t="inlineStr">
         <is>
-          <t>M&amp;M'S Pinda chocolade snoepjes 125g</t>
+          <t>M&amp;M'S Salted caramel chocolade snoepjes maxi 367g</t>
         </is>
       </c>
       <c r="B69" t="inlineStr">
@@ -2911,12 +2911,12 @@
       </c>
       <c r="C69" t="inlineStr">
         <is>
-          <t>2,08</t>
+          <t>5,93</t>
         </is>
       </c>
       <c r="D69" t="inlineStr">
         <is>
-          <t>125 g</t>
+          <t>367 g</t>
         </is>
       </c>
       <c r="E69" t="inlineStr">
@@ -2931,14 +2931,14 @@
       </c>
       <c r="G69" t="inlineStr">
         <is>
-          <t>2025-07-07</t>
+          <t>2025-07-21</t>
         </is>
       </c>
     </row>
     <row r="70">
       <c r="A70" t="inlineStr">
         <is>
-          <t>M&amp;M'S Salted caramel chocolade snoepjes maxi 367g</t>
+          <t>M&amp;M'S Choco chocolade snoepjes 125g</t>
         </is>
       </c>
       <c r="B70" t="inlineStr">
@@ -2948,12 +2948,12 @@
       </c>
       <c r="C70" t="inlineStr">
         <is>
-          <t>5,53</t>
+          <t>2,09</t>
         </is>
       </c>
       <c r="D70" t="inlineStr">
         <is>
-          <t>367 g</t>
+          <t>125 g</t>
         </is>
       </c>
       <c r="E70" t="inlineStr">
@@ -2968,14 +2968,14 @@
       </c>
       <c r="G70" t="inlineStr">
         <is>
-          <t>2025-07-07</t>
+          <t>2025-07-21</t>
         </is>
       </c>
     </row>
     <row r="71">
       <c r="A71" t="inlineStr">
         <is>
-          <t>M&amp;M'S Salted caramel chocolade snoepjes 176g</t>
+          <t>M&amp;M'S Crispy chocolade snoepjes 107g</t>
         </is>
       </c>
       <c r="B71" t="inlineStr">
@@ -2985,12 +2985,12 @@
       </c>
       <c r="C71" t="inlineStr">
         <is>
-          <t>2,68</t>
+          <t>2,08</t>
         </is>
       </c>
       <c r="D71" t="inlineStr">
         <is>
-          <t>176 g</t>
+          <t>107 g</t>
         </is>
       </c>
       <c r="E71" t="inlineStr">
@@ -3005,14 +3005,14 @@
       </c>
       <c r="G71" t="inlineStr">
         <is>
-          <t>2025-07-07</t>
+          <t>2025-07-21</t>
         </is>
       </c>
     </row>
     <row r="72">
       <c r="A72" t="inlineStr">
         <is>
-          <t>M&amp;M'S Crispy chocolade snoepjes 107g</t>
+          <t>M&amp;M'S Choco chocolade snoepjes 200g</t>
         </is>
       </c>
       <c r="B72" t="inlineStr">
@@ -3022,12 +3022,12 @@
       </c>
       <c r="C72" t="inlineStr">
         <is>
-          <t>2,08</t>
+          <t>3,08</t>
         </is>
       </c>
       <c r="D72" t="inlineStr">
         <is>
-          <t>107 g</t>
+          <t>200 g</t>
         </is>
       </c>
       <c r="E72" t="inlineStr">
@@ -3042,14 +3042,14 @@
       </c>
       <c r="G72" t="inlineStr">
         <is>
-          <t>2025-07-07</t>
+          <t>2025-07-21</t>
         </is>
       </c>
     </row>
     <row r="73">
       <c r="A73" t="inlineStr">
         <is>
-          <t>M&amp;M'S Minis chocolade snoepjes 176g</t>
+          <t>M&amp;M'S Salted caramel chocolade snoepjes 176g</t>
         </is>
       </c>
       <c r="B73" t="inlineStr">
@@ -3059,7 +3059,7 @@
       </c>
       <c r="C73" t="inlineStr">
         <is>
-          <t>3,08</t>
+          <t>2,89</t>
         </is>
       </c>
       <c r="D73" t="inlineStr">
@@ -3079,14 +3079,14 @@
       </c>
       <c r="G73" t="inlineStr">
         <is>
-          <t>2025-07-07</t>
+          <t>2025-07-21</t>
         </is>
       </c>
     </row>
     <row r="74">
       <c r="A74" t="inlineStr">
         <is>
-          <t>M&amp;M's Mini Cookie 180g</t>
+          <t>M&amp;M'S Minis chocolade snoepjes 176g</t>
         </is>
       </c>
       <c r="B74" t="inlineStr">
@@ -3096,12 +3096,12 @@
       </c>
       <c r="C74" t="inlineStr">
         <is>
-          <t>2,69</t>
+          <t>3,08</t>
         </is>
       </c>
       <c r="D74" t="inlineStr">
         <is>
-          <t>Weight not found</t>
+          <t>176 g</t>
         </is>
       </c>
       <c r="E74" t="inlineStr">
@@ -3116,44 +3116,477 @@
       </c>
       <c r="G74" t="inlineStr">
         <is>
-          <t>2025-07-07</t>
+          <t>2025-07-21</t>
         </is>
       </c>
     </row>
     <row r="75">
       <c r="A75" t="inlineStr">
         <is>
+          <t>mini's M&amp;M’s®  Cookies</t>
+        </is>
+      </c>
+      <c r="B75" t="inlineStr">
+        <is>
+          <t>Promo price not found</t>
+        </is>
+      </c>
+      <c r="C75" t="inlineStr">
+        <is>
+          <t>2,69</t>
+        </is>
+      </c>
+      <c r="D75" t="inlineStr">
+        <is>
+          <t>180 g</t>
+        </is>
+      </c>
+      <c r="E75" t="inlineStr">
+        <is>
+          <t>branded</t>
+        </is>
+      </c>
+      <c r="F75" t="inlineStr">
+        <is>
+          <t>Jumbo</t>
+        </is>
+      </c>
+      <c r="G75" t="inlineStr">
+        <is>
+          <t>2025-07-21</t>
+        </is>
+      </c>
+    </row>
+    <row r="76">
+      <c r="A76" t="inlineStr">
+        <is>
           <t>M&amp;M'S Minis chocolade snoepjes maxi 360g</t>
         </is>
       </c>
-      <c r="B75" t="inlineStr">
-        <is>
-          <t>Promo price not found</t>
-        </is>
-      </c>
-      <c r="C75" t="inlineStr">
+      <c r="B76" t="inlineStr">
+        <is>
+          <t>Promo price not found</t>
+        </is>
+      </c>
+      <c r="C76" t="inlineStr">
         <is>
           <t>5,99</t>
         </is>
       </c>
-      <c r="D75" t="inlineStr">
+      <c r="D76" t="inlineStr">
         <is>
           <t>Weight not found</t>
         </is>
       </c>
-      <c r="E75" t="inlineStr">
+      <c r="E76" t="inlineStr">
         <is>
           <t>branded</t>
         </is>
       </c>
-      <c r="F75" t="inlineStr">
+      <c r="F76" t="inlineStr">
         <is>
           <t>Jumbo</t>
         </is>
       </c>
-      <c r="G75" t="inlineStr">
-        <is>
-          <t>2025-07-07</t>
+      <c r="G76" t="inlineStr">
+        <is>
+          <t>2025-07-21</t>
+        </is>
+      </c>
+    </row>
+    <row r="77">
+      <c r="A77" t="inlineStr">
+        <is>
+          <t xml:space="preserve">M&amp;M'S Melk Chocolade Pinda </t>
+        </is>
+      </c>
+      <c r="B77" t="inlineStr">
+        <is>
+          <t>2.29</t>
+        </is>
+      </c>
+      <c r="C77" t="inlineStr"/>
+      <c r="D77" t="inlineStr">
+        <is>
+          <t>Per 125 g</t>
+        </is>
+      </c>
+      <c r="E77" t="inlineStr">
+        <is>
+          <t>branded</t>
+        </is>
+      </c>
+      <c r="F77" t="inlineStr">
+        <is>
+          <t>Plus</t>
+        </is>
+      </c>
+      <c r="G77" t="inlineStr">
+        <is>
+          <t>2025-07-21</t>
+        </is>
+      </c>
+    </row>
+    <row r="78">
+      <c r="A78" t="inlineStr">
+        <is>
+          <t xml:space="preserve">M&amp;M'S Melk Chocolade Choco </t>
+        </is>
+      </c>
+      <c r="B78" t="inlineStr">
+        <is>
+          <t>2.29</t>
+        </is>
+      </c>
+      <c r="C78" t="inlineStr"/>
+      <c r="D78" t="inlineStr">
+        <is>
+          <t>Per 125 g</t>
+        </is>
+      </c>
+      <c r="E78" t="inlineStr">
+        <is>
+          <t>branded</t>
+        </is>
+      </c>
+      <c r="F78" t="inlineStr">
+        <is>
+          <t>Plus</t>
+        </is>
+      </c>
+      <c r="G78" t="inlineStr">
+        <is>
+          <t>2025-07-21</t>
+        </is>
+      </c>
+    </row>
+    <row r="79">
+      <c r="A79" t="inlineStr">
+        <is>
+          <t>M&amp;M'S Chocolade snoepjes zakje</t>
+        </is>
+      </c>
+      <c r="B79" t="inlineStr">
+        <is>
+          <t>1.49</t>
+        </is>
+      </c>
+      <c r="C79" t="inlineStr"/>
+      <c r="D79" t="inlineStr">
+        <is>
+          <t>Per 100 g</t>
+        </is>
+      </c>
+      <c r="E79" t="inlineStr">
+        <is>
+          <t>branded</t>
+        </is>
+      </c>
+      <c r="F79" t="inlineStr">
+        <is>
+          <t>Plus</t>
+        </is>
+      </c>
+      <c r="G79" t="inlineStr">
+        <is>
+          <t>2025-07-21</t>
+        </is>
+      </c>
+    </row>
+    <row r="80">
+      <c r="A80" t="inlineStr">
+        <is>
+          <t>M&amp;M'S Melk chocolade karamel snoepjes</t>
+        </is>
+      </c>
+      <c r="B80" t="inlineStr">
+        <is>
+          <t>5.99</t>
+        </is>
+      </c>
+      <c r="C80" t="inlineStr"/>
+      <c r="D80" t="inlineStr">
+        <is>
+          <t>Per 367 g</t>
+        </is>
+      </c>
+      <c r="E80" t="inlineStr">
+        <is>
+          <t>branded</t>
+        </is>
+      </c>
+      <c r="F80" t="inlineStr">
+        <is>
+          <t>Plus</t>
+        </is>
+      </c>
+      <c r="G80" t="inlineStr">
+        <is>
+          <t>2025-07-21</t>
+        </is>
+      </c>
+    </row>
+    <row r="81">
+      <c r="A81" t="inlineStr">
+        <is>
+          <t xml:space="preserve">M&amp;M'S Crispy Melk Chocolade </t>
+        </is>
+      </c>
+      <c r="B81" t="inlineStr">
+        <is>
+          <t>1.49</t>
+        </is>
+      </c>
+      <c r="C81" t="inlineStr"/>
+      <c r="D81" t="inlineStr">
+        <is>
+          <t>Per 77 g</t>
+        </is>
+      </c>
+      <c r="E81" t="inlineStr">
+        <is>
+          <t>branded</t>
+        </is>
+      </c>
+      <c r="F81" t="inlineStr">
+        <is>
+          <t>Plus</t>
+        </is>
+      </c>
+      <c r="G81" t="inlineStr">
+        <is>
+          <t>2025-07-21</t>
+        </is>
+      </c>
+    </row>
+    <row r="82">
+      <c r="A82" t="inlineStr">
+        <is>
+          <t>M&amp;M'S Peanut</t>
+        </is>
+      </c>
+      <c r="B82" t="inlineStr">
+        <is>
+          <t>9.99</t>
+        </is>
+      </c>
+      <c r="C82" t="inlineStr"/>
+      <c r="D82" t="inlineStr">
+        <is>
+          <t>Per 800 g</t>
+        </is>
+      </c>
+      <c r="E82" t="inlineStr">
+        <is>
+          <t>branded</t>
+        </is>
+      </c>
+      <c r="F82" t="inlineStr">
+        <is>
+          <t>Plus</t>
+        </is>
+      </c>
+      <c r="G82" t="inlineStr">
+        <is>
+          <t>2025-07-21</t>
+        </is>
+      </c>
+    </row>
+    <row r="83">
+      <c r="A83" t="inlineStr">
+        <is>
+          <t>M&amp;M'S Pinda chocolade snoepjes zakje</t>
+        </is>
+      </c>
+      <c r="B83" t="inlineStr">
+        <is>
+          <t>1.20</t>
+        </is>
+      </c>
+      <c r="C83" t="inlineStr"/>
+      <c r="D83" t="inlineStr">
+        <is>
+          <t>Per 82 g</t>
+        </is>
+      </c>
+      <c r="E83" t="inlineStr">
+        <is>
+          <t>branded</t>
+        </is>
+      </c>
+      <c r="F83" t="inlineStr">
+        <is>
+          <t>Plus</t>
+        </is>
+      </c>
+      <c r="G83" t="inlineStr">
+        <is>
+          <t>2025-07-21</t>
+        </is>
+      </c>
+    </row>
+    <row r="84">
+      <c r="A84" t="inlineStr">
+        <is>
+          <t>M&amp;M'S Melk chocolade pinda snoepjes</t>
+        </is>
+      </c>
+      <c r="B84" t="inlineStr">
+        <is>
+          <t>5.69</t>
+        </is>
+      </c>
+      <c r="C84" t="inlineStr"/>
+      <c r="D84" t="inlineStr">
+        <is>
+          <t>Per 400 g</t>
+        </is>
+      </c>
+      <c r="E84" t="inlineStr">
+        <is>
+          <t>branded</t>
+        </is>
+      </c>
+      <c r="F84" t="inlineStr">
+        <is>
+          <t>Plus</t>
+        </is>
+      </c>
+      <c r="G84" t="inlineStr">
+        <is>
+          <t>2025-07-21</t>
+        </is>
+      </c>
+    </row>
+    <row r="85">
+      <c r="A85" t="inlineStr">
+        <is>
+          <t xml:space="preserve">M&amp;M'S Melk Chocolade Crispy </t>
+        </is>
+      </c>
+      <c r="B85" t="inlineStr">
+        <is>
+          <t>2.29</t>
+        </is>
+      </c>
+      <c r="C85" t="inlineStr"/>
+      <c r="D85" t="inlineStr">
+        <is>
+          <t>Per 107 g</t>
+        </is>
+      </c>
+      <c r="E85" t="inlineStr">
+        <is>
+          <t>branded</t>
+        </is>
+      </c>
+      <c r="F85" t="inlineStr">
+        <is>
+          <t>Plus</t>
+        </is>
+      </c>
+      <c r="G85" t="inlineStr">
+        <is>
+          <t>2025-07-21</t>
+        </is>
+      </c>
+    </row>
+    <row r="86">
+      <c r="A86" t="inlineStr">
+        <is>
+          <t>M&amp;M'S Melk chocolade choco snoepjes zak</t>
+        </is>
+      </c>
+      <c r="B86" t="inlineStr">
+        <is>
+          <t>5.69</t>
+        </is>
+      </c>
+      <c r="C86" t="inlineStr"/>
+      <c r="D86" t="inlineStr">
+        <is>
+          <t>Per 400 g</t>
+        </is>
+      </c>
+      <c r="E86" t="inlineStr">
+        <is>
+          <t>branded</t>
+        </is>
+      </c>
+      <c r="F86" t="inlineStr">
+        <is>
+          <t>Plus</t>
+        </is>
+      </c>
+      <c r="G86" t="inlineStr">
+        <is>
+          <t>2025-07-21</t>
+        </is>
+      </c>
+    </row>
+    <row r="87">
+      <c r="A87" t="inlineStr">
+        <is>
+          <t>M&amp;M'S Melk Chocolade Crispy</t>
+        </is>
+      </c>
+      <c r="B87" t="inlineStr">
+        <is>
+          <t>5.69</t>
+        </is>
+      </c>
+      <c r="C87" t="inlineStr"/>
+      <c r="D87" t="inlineStr">
+        <is>
+          <t>Per 340 g</t>
+        </is>
+      </c>
+      <c r="E87" t="inlineStr">
+        <is>
+          <t>branded</t>
+        </is>
+      </c>
+      <c r="F87" t="inlineStr">
+        <is>
+          <t>Plus</t>
+        </is>
+      </c>
+      <c r="G87" t="inlineStr">
+        <is>
+          <t>2025-07-21</t>
+        </is>
+      </c>
+    </row>
+    <row r="88">
+      <c r="A88" t="inlineStr">
+        <is>
+          <t>M&amp;M'S Pinda chocolade snoepjes zak</t>
+        </is>
+      </c>
+      <c r="B88" t="inlineStr">
+        <is>
+          <t>3.39</t>
+        </is>
+      </c>
+      <c r="C88" t="inlineStr"/>
+      <c r="D88" t="inlineStr">
+        <is>
+          <t>Per 200 g</t>
+        </is>
+      </c>
+      <c r="E88" t="inlineStr">
+        <is>
+          <t>branded</t>
+        </is>
+      </c>
+      <c r="F88" t="inlineStr">
+        <is>
+          <t>Plus</t>
+        </is>
+      </c>
+      <c r="G88" t="inlineStr">
+        <is>
+          <t>2025-07-21</t>
         </is>
       </c>
     </row>
@@ -3168,7 +3601,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G49"/>
+  <dimension ref="A1:G50"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -3246,7 +3679,7 @@
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>2025-07-07</t>
+          <t>2025-07-21</t>
         </is>
       </c>
     </row>
@@ -3283,7 +3716,7 @@
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>2025-07-07</t>
+          <t>2025-07-21</t>
         </is>
       </c>
     </row>
@@ -3320,7 +3753,7 @@
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>2025-07-07</t>
+          <t>2025-07-21</t>
         </is>
       </c>
     </row>
@@ -3357,7 +3790,7 @@
       </c>
       <c r="G5" t="inlineStr">
         <is>
-          <t>2025-07-07</t>
+          <t>2025-07-21</t>
         </is>
       </c>
     </row>
@@ -3394,7 +3827,7 @@
       </c>
       <c r="G6" t="inlineStr">
         <is>
-          <t>2025-07-07</t>
+          <t>2025-07-21</t>
         </is>
       </c>
     </row>
@@ -3431,7 +3864,7 @@
       </c>
       <c r="G7" t="inlineStr">
         <is>
-          <t>2025-07-07</t>
+          <t>2025-07-21</t>
         </is>
       </c>
     </row>
@@ -3468,7 +3901,7 @@
       </c>
       <c r="G8" t="inlineStr">
         <is>
-          <t>2025-07-07</t>
+          <t>2025-07-21</t>
         </is>
       </c>
     </row>
@@ -3505,7 +3938,7 @@
       </c>
       <c r="G9" t="inlineStr">
         <is>
-          <t>2025-07-07</t>
+          <t>2025-07-21</t>
         </is>
       </c>
     </row>
@@ -3542,7 +3975,7 @@
       </c>
       <c r="G10" t="inlineStr">
         <is>
-          <t>2025-07-07</t>
+          <t>2025-07-21</t>
         </is>
       </c>
     </row>
@@ -3579,29 +4012,29 @@
       </c>
       <c r="G11" t="inlineStr">
         <is>
-          <t>2025-07-07</t>
+          <t>2025-07-21</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>Bekijk AH Chocobites disco dip &amp; pretzel</t>
+          <t>Bekijk AH Pindarotsjes wit</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>2.49</t>
+          <t>2.59</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>2.49</t>
+          <t>2.59</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>125 g</t>
+          <t>250 g</t>
         </is>
       </c>
       <c r="E12" t="inlineStr">
@@ -3616,29 +4049,29 @@
       </c>
       <c r="G12" t="inlineStr">
         <is>
-          <t>2025-07-07</t>
+          <t>2025-07-21</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>Bekijk AH Pindarotsjes wit</t>
+          <t>Bekijk AH Chocobites disco dip &amp; pretzel</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>2.59</t>
+          <t>2.49</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>2.59</t>
+          <t>2.49</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>250 g</t>
+          <t>125 g</t>
         </is>
       </c>
       <c r="E13" t="inlineStr">
@@ -3653,7 +4086,7 @@
       </c>
       <c r="G13" t="inlineStr">
         <is>
-          <t>2025-07-07</t>
+          <t>2025-07-21</t>
         </is>
       </c>
     </row>
@@ -3690,14 +4123,14 @@
       </c>
       <c r="G14" t="inlineStr">
         <is>
-          <t>2025-07-07</t>
+          <t>2025-07-21</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>Bekijk AH Chocobites koek &amp; knettersuiker</t>
+          <t>Bekijk AH Chocobites crispy corn &amp; choco trio</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
@@ -3727,14 +4160,14 @@
       </c>
       <c r="G15" t="inlineStr">
         <is>
-          <t>2025-07-07</t>
+          <t>2025-07-21</t>
         </is>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>Bekijk AH Chocobites crispy corn &amp; choco trio</t>
+          <t>Bekijk AH Chocobites koek &amp; knettersuiker</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
@@ -3764,7 +4197,7 @@
       </c>
       <c r="G16" t="inlineStr">
         <is>
-          <t>2025-07-07</t>
+          <t>2025-07-21</t>
         </is>
       </c>
     </row>
@@ -3801,7 +4234,7 @@
       </c>
       <c r="G17" t="inlineStr">
         <is>
-          <t>2025-07-07</t>
+          <t>2025-07-21</t>
         </is>
       </c>
     </row>
@@ -3838,7 +4271,7 @@
       </c>
       <c r="G18" t="inlineStr">
         <is>
-          <t>2025-07-07</t>
+          <t>2025-07-21</t>
         </is>
       </c>
     </row>
@@ -3875,14 +4308,14 @@
       </c>
       <c r="G19" t="inlineStr">
         <is>
-          <t>2025-07-07</t>
+          <t>2025-07-21</t>
         </is>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>Bekijk AH Stroopwafelrotsjes</t>
+          <t>Bekijk AH Chocolade blaadjes puur citroen</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
@@ -3912,24 +4345,24 @@
       </c>
       <c r="G20" t="inlineStr">
         <is>
-          <t>2025-07-07</t>
+          <t>2025-07-21</t>
         </is>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>Bekijk AH Chocobites zwarte bes &amp; cheesecakesmaak</t>
+          <t>Bekijk AH Stroopwafelrotsjes</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>2.59</t>
+          <t>2.99</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>2.59</t>
+          <t>2.99</t>
         </is>
       </c>
       <c r="D21" t="inlineStr">
@@ -3949,24 +4382,24 @@
       </c>
       <c r="G21" t="inlineStr">
         <is>
-          <t>2025-07-07</t>
+          <t>2025-07-21</t>
         </is>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>Bekijk AH Chocolade blaadjes puur citroen</t>
+          <t>Bekijk AH Chocobites zwarte bes &amp; cheesecakesmaak</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>2.99</t>
+          <t>2.59</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>2.99</t>
+          <t>2.59</t>
         </is>
       </c>
       <c r="D22" t="inlineStr">
@@ -3986,7 +4419,7 @@
       </c>
       <c r="G22" t="inlineStr">
         <is>
-          <t>2025-07-07</t>
+          <t>2025-07-21</t>
         </is>
       </c>
     </row>
@@ -4023,7 +4456,7 @@
       </c>
       <c r="G23" t="inlineStr">
         <is>
-          <t>2025-07-07</t>
+          <t>2025-07-21</t>
         </is>
       </c>
     </row>
@@ -4060,29 +4493,29 @@
       </c>
       <c r="G24" t="inlineStr">
         <is>
-          <t>2025-07-07</t>
+          <t>2025-07-21</t>
         </is>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>Bekijk AH Pinda choco's</t>
+          <t>Bekijk AH Koffieboontjes pure chocolade</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>2.69</t>
+          <t>2.99</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>2.69</t>
+          <t>2.99</t>
         </is>
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>400 g</t>
+          <t>125 g</t>
         </is>
       </c>
       <c r="E25" t="inlineStr">
@@ -4097,29 +4530,29 @@
       </c>
       <c r="G25" t="inlineStr">
         <is>
-          <t>2025-07-07</t>
+          <t>2025-07-21</t>
         </is>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>Bekijk AH Rozijn choco's</t>
+          <t>Bekijk AH Pinda choco's</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>1.69</t>
+          <t>2.69</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>1.69</t>
+          <t>2.69</t>
         </is>
       </c>
       <c r="D26" t="inlineStr">
         <is>
-          <t>200 g</t>
+          <t>400 g</t>
         </is>
       </c>
       <c r="E26" t="inlineStr">
@@ -4134,24 +4567,24 @@
       </c>
       <c r="G26" t="inlineStr">
         <is>
-          <t>2025-07-07</t>
+          <t>2025-07-21</t>
         </is>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>Bekijk AH Hazelnoten choco's</t>
+          <t>Bekijk AH Rozijn choco's</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>2.19</t>
+          <t>1.69</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>2.19</t>
+          <t>1.69</t>
         </is>
       </c>
       <c r="D27" t="inlineStr">
@@ -4171,24 +4604,24 @@
       </c>
       <c r="G27" t="inlineStr">
         <is>
-          <t>2025-07-07</t>
+          <t>2025-07-21</t>
         </is>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>Bekijk AH Choco pinda's zoet</t>
+          <t>Bekijk AH Hazelnoten choco's</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>1.79</t>
+          <t>2.19</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>1.79</t>
+          <t>2.19</t>
         </is>
       </c>
       <c r="D28" t="inlineStr">
@@ -4208,24 +4641,24 @@
       </c>
       <c r="G28" t="inlineStr">
         <is>
-          <t>2025-07-07</t>
+          <t>2025-07-21</t>
         </is>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>Bekijk AH Terra Walnoten ongebrand</t>
+          <t>Bekijk AH Choco pinda's zoet</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>3.29</t>
+          <t>1.79</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>3.29</t>
+          <t>1.79</t>
         </is>
       </c>
       <c r="D29" t="inlineStr">
@@ -4245,29 +4678,29 @@
       </c>
       <c r="G29" t="inlineStr">
         <is>
-          <t>2025-07-07</t>
+          <t>2025-07-21</t>
         </is>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>Bekijk AH Walnoten ongebrand 2-pack</t>
+          <t>Bekijk AH Terra Walnoten ongebrand</t>
         </is>
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>Oude prijs: €6.58</t>
+          <t>3.29</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>6.25</t>
+          <t>3.29</t>
         </is>
       </c>
       <c r="D30" t="inlineStr">
         <is>
-          <t>2 stuks</t>
+          <t>200 g</t>
         </is>
       </c>
       <c r="E30" t="inlineStr">
@@ -4282,29 +4715,29 @@
       </c>
       <c r="G30" t="inlineStr">
         <is>
-          <t>2025-07-07</t>
+          <t>2025-07-21</t>
         </is>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>Bekijk AH Cashewnoten ongezouten</t>
+          <t>Bekijk AH Walnoten ongebrand 2-pack</t>
         </is>
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>3.19</t>
+          <t>Oude prijs: €6.58</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>3.19</t>
+          <t>6.25</t>
         </is>
       </c>
       <c r="D31" t="inlineStr">
         <is>
-          <t>250 g</t>
+          <t>2 stuks</t>
         </is>
       </c>
       <c r="E31" t="inlineStr">
@@ -4319,29 +4752,29 @@
       </c>
       <c r="G31" t="inlineStr">
         <is>
-          <t>2025-07-07</t>
+          <t>2025-07-21</t>
         </is>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>Bekijk AH Macadamiamix gezouten</t>
+          <t>Bekijk AH Cashewnoten ongezouten</t>
         </is>
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>2.69</t>
+          <t>3.19</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>2.69</t>
+          <t>3.19</t>
         </is>
       </c>
       <c r="D32" t="inlineStr">
         <is>
-          <t>100 g</t>
+          <t>250 g</t>
         </is>
       </c>
       <c r="E32" t="inlineStr">
@@ -4356,34 +4789,34 @@
       </c>
       <c r="G32" t="inlineStr">
         <is>
-          <t>2025-07-07</t>
+          <t>2025-07-21</t>
         </is>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>Bekijk M&amp;M'S Pinda melk chocolade maxi</t>
+          <t>Bekijk AH Macadamiamix gezouten</t>
         </is>
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>5.69</t>
+          <t>2.69</t>
         </is>
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>5.69</t>
+          <t>2.69</t>
         </is>
       </c>
       <c r="D33" t="inlineStr">
         <is>
-          <t>400 g</t>
+          <t>100 g</t>
         </is>
       </c>
       <c r="E33" t="inlineStr">
         <is>
-          <t>Branded</t>
+          <t>Non_Branded</t>
         </is>
       </c>
       <c r="F33" t="inlineStr">
@@ -4393,7 +4826,7 @@
       </c>
       <c r="G33" t="inlineStr">
         <is>
-          <t>2025-07-07</t>
+          <t>2025-07-21</t>
         </is>
       </c>
     </row>
@@ -4430,14 +4863,14 @@
       </c>
       <c r="G34" t="inlineStr">
         <is>
-          <t>2025-07-07</t>
+          <t>2025-07-21</t>
         </is>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>Bekijk M&amp;M'S Melk chocolade</t>
+          <t>Bekijk M&amp;M'S Pinda melk chocolade maxi</t>
         </is>
       </c>
       <c r="B35" t="inlineStr">
@@ -4467,7 +4900,7 @@
       </c>
       <c r="G35" t="inlineStr">
         <is>
-          <t>2025-07-07</t>
+          <t>2025-07-21</t>
         </is>
       </c>
     </row>
@@ -4504,7 +4937,7 @@
       </c>
       <c r="G36" t="inlineStr">
         <is>
-          <t>2025-07-07</t>
+          <t>2025-07-21</t>
         </is>
       </c>
     </row>
@@ -4541,14 +4974,14 @@
       </c>
       <c r="G37" t="inlineStr">
         <is>
-          <t>2025-07-07</t>
+          <t>2025-07-21</t>
         </is>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>Bekijk M&amp;M'S Crispy melkchocolade maxi</t>
+          <t>Bekijk M&amp;M'S Melk chocolade</t>
         </is>
       </c>
       <c r="B38" t="inlineStr">
@@ -4563,7 +4996,7 @@
       </c>
       <c r="D38" t="inlineStr">
         <is>
-          <t>340 g</t>
+          <t>400 g</t>
         </is>
       </c>
       <c r="E38" t="inlineStr">
@@ -4578,29 +5011,29 @@
       </c>
       <c r="G38" t="inlineStr">
         <is>
-          <t>2025-07-07</t>
+          <t>2025-07-21</t>
         </is>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>Bekijk M&amp;M'S Gezouten karamel melk chocolade</t>
+          <t>Bekijk M&amp;M'S Crispy melkchocolade maxi</t>
         </is>
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>2.95</t>
+          <t>5.69</t>
         </is>
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>2.95</t>
+          <t>5.69</t>
         </is>
       </c>
       <c r="D39" t="inlineStr">
         <is>
-          <t>176 g</t>
+          <t>340 g</t>
         </is>
       </c>
       <c r="E39" t="inlineStr">
@@ -4615,29 +5048,29 @@
       </c>
       <c r="G39" t="inlineStr">
         <is>
-          <t>2025-07-07</t>
+          <t>2025-07-21</t>
         </is>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>Bekijk M&amp;M'S Gezouten karamel melk chocolade maxi</t>
+          <t>Bekijk M&amp;M'S Gezouten karamel melk chocolade</t>
         </is>
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>5.99</t>
+          <t>2.95</t>
         </is>
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>5.99</t>
+          <t>2.95</t>
         </is>
       </c>
       <c r="D40" t="inlineStr">
         <is>
-          <t>367 g</t>
+          <t>176 g</t>
         </is>
       </c>
       <c r="E40" t="inlineStr">
@@ -4652,29 +5085,29 @@
       </c>
       <c r="G40" t="inlineStr">
         <is>
-          <t>2025-07-07</t>
+          <t>2025-07-21</t>
         </is>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>Bekijk M&amp;M'S Pinda melk chocolade</t>
+          <t>Bekijk M&amp;M'S Minis melk chocolade</t>
         </is>
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>2.29</t>
+          <t>3.39</t>
         </is>
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>2.29</t>
+          <t>3.39</t>
         </is>
       </c>
       <c r="D41" t="inlineStr">
         <is>
-          <t>125 g</t>
+          <t>176 g</t>
         </is>
       </c>
       <c r="E41" t="inlineStr">
@@ -4689,29 +5122,29 @@
       </c>
       <c r="G41" t="inlineStr">
         <is>
-          <t>2025-07-07</t>
+          <t>2025-07-21</t>
         </is>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>Bekijk M&amp;M'S Minis melk chocolade</t>
+          <t>Bekijk M&amp;M'S Gezouten karamel melk chocolade maxi</t>
         </is>
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>3.39</t>
+          <t>5.99</t>
         </is>
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>3.39</t>
+          <t>5.99</t>
         </is>
       </c>
       <c r="D42" t="inlineStr">
         <is>
-          <t>176 g</t>
+          <t>367 g</t>
         </is>
       </c>
       <c r="E42" t="inlineStr">
@@ -4726,14 +5159,14 @@
       </c>
       <c r="G42" t="inlineStr">
         <is>
-          <t>2025-07-07</t>
+          <t>2025-07-21</t>
         </is>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>Bekijk M&amp;M'S Melk chocolade</t>
+          <t>Bekijk M&amp;M'S Pinda melk chocolade</t>
         </is>
       </c>
       <c r="B43" t="inlineStr">
@@ -4763,7 +5196,7 @@
       </c>
       <c r="G43" t="inlineStr">
         <is>
-          <t>2025-07-07</t>
+          <t>2025-07-21</t>
         </is>
       </c>
     </row>
@@ -4780,7 +5213,7 @@
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>7.00</t>
+          <t>6.99</t>
         </is>
       </c>
       <c r="D44" t="inlineStr">
@@ -4800,14 +5233,14 @@
       </c>
       <c r="G44" t="inlineStr">
         <is>
-          <t>2025-07-07</t>
+          <t>2025-07-21</t>
         </is>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>Bekijk M&amp;M'S Crispy melk chocolade</t>
+          <t>Bekijk M&amp;M'S Melk chocolade</t>
         </is>
       </c>
       <c r="B45" t="inlineStr">
@@ -4822,7 +5255,7 @@
       </c>
       <c r="D45" t="inlineStr">
         <is>
-          <t>107 g</t>
+          <t>125 g</t>
         </is>
       </c>
       <c r="E45" t="inlineStr">
@@ -4837,7 +5270,7 @@
       </c>
       <c r="G45" t="inlineStr">
         <is>
-          <t>2025-07-07</t>
+          <t>2025-07-21</t>
         </is>
       </c>
     </row>
@@ -4874,29 +5307,29 @@
       </c>
       <c r="G46" t="inlineStr">
         <is>
-          <t>2025-07-07</t>
+          <t>2025-07-21</t>
         </is>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>Bekijk M&amp;M'S Chocolade party</t>
+          <t>Bekijk M&amp;M'S Crispy melk chocolade</t>
         </is>
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>9.99</t>
+          <t>2.29</t>
         </is>
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>9.99</t>
+          <t>2.29</t>
         </is>
       </c>
       <c r="D47" t="inlineStr">
         <is>
-          <t>800 g</t>
+          <t>107 g</t>
         </is>
       </c>
       <c r="E47" t="inlineStr">
@@ -4911,14 +5344,14 @@
       </c>
       <c r="G47" t="inlineStr">
         <is>
-          <t>2025-07-07</t>
+          <t>2025-07-21</t>
         </is>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>Bekijk M&amp;M'S Crispy chocolade party</t>
+          <t>Bekijk M&amp;M'S Chocolade party</t>
         </is>
       </c>
       <c r="B48" t="inlineStr">
@@ -4933,7 +5366,7 @@
       </c>
       <c r="D48" t="inlineStr">
         <is>
-          <t>675 g</t>
+          <t>800 g</t>
         </is>
       </c>
       <c r="E48" t="inlineStr">
@@ -4948,44 +5381,81 @@
       </c>
       <c r="G48" t="inlineStr">
         <is>
-          <t>2025-07-07</t>
+          <t>2025-07-21</t>
         </is>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
+          <t>Bekijk M&amp;M'S Crispy chocolade party</t>
+        </is>
+      </c>
+      <c r="B49" t="inlineStr">
+        <is>
+          <t>9.99</t>
+        </is>
+      </c>
+      <c r="C49" t="inlineStr">
+        <is>
+          <t>9.99</t>
+        </is>
+      </c>
+      <c r="D49" t="inlineStr">
+        <is>
+          <t>675 g</t>
+        </is>
+      </c>
+      <c r="E49" t="inlineStr">
+        <is>
+          <t>Branded</t>
+        </is>
+      </c>
+      <c r="F49" t="inlineStr">
+        <is>
+          <t>AH</t>
+        </is>
+      </c>
+      <c r="G49" t="inlineStr">
+        <is>
+          <t>2025-07-21</t>
+        </is>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" t="inlineStr">
+        <is>
           <t>Bekijk M&amp;M'S Pinda melk chocolade</t>
         </is>
       </c>
-      <c r="B49" t="inlineStr">
+      <c r="B50" t="inlineStr">
         <is>
           <t>1.49</t>
         </is>
       </c>
-      <c r="C49" t="inlineStr">
+      <c r="C50" t="inlineStr">
         <is>
           <t>1.49</t>
         </is>
       </c>
-      <c r="D49" t="inlineStr">
+      <c r="D50" t="inlineStr">
         <is>
           <t>45 g</t>
         </is>
       </c>
-      <c r="E49" t="inlineStr">
+      <c r="E50" t="inlineStr">
         <is>
           <t>Branded</t>
         </is>
       </c>
-      <c r="F49" t="inlineStr">
+      <c r="F50" t="inlineStr">
         <is>
           <t>AH</t>
         </is>
       </c>
-      <c r="G49" t="inlineStr">
-        <is>
-          <t>2025-07-07</t>
+      <c r="G50" t="inlineStr">
+        <is>
+          <t>2025-07-21</t>
         </is>
       </c>
     </row>

</xml_diff>